<commit_message>
Rezolvare canal de pana
- trebuie realizat arborele
</commit_message>
<xml_diff>
--- a/PROIECT OM2 CALCULE.xlsx
+++ b/PROIECT OM2 CALCULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Reductor-Conico-Cilindric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCE2CE0-50AD-44C5-B501-F293A5805284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCBF37B-EA3B-487F-B3CB-6C84493B2700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="182">
   <si>
     <t>[kW]</t>
   </si>
@@ -1252,12 +1252,103 @@
   <si>
     <t>nl2</t>
   </si>
+  <si>
+    <t>Date intrare arbore intrare</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>grosimea coroanei (g)</t>
+  </si>
+  <si>
+    <t>βm</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>Lp</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>Date de intrare arbore median</t>
+  </si>
+  <si>
+    <t>Date de intrare arbore iesire</t>
+  </si>
+  <si>
+    <t>b pana</t>
+  </si>
+  <si>
+    <t>x1 C</t>
+  </si>
+  <si>
+    <t>x1 A</t>
+  </si>
+  <si>
+    <t>δ2</t>
+  </si>
+  <si>
+    <t>δ3</t>
+  </si>
+  <si>
+    <t>δ4</t>
+  </si>
+  <si>
+    <t>δ5</t>
+  </si>
+  <si>
+    <t>Arbore de intrare și pinionul conic separate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.00000;[Red]0.00000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
@@ -1433,7 +1524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1562,8 +1653,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1767,8 +1870,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
@@ -1777,8 +1900,9 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2010,6 +2134,63 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="17" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="17" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2022,9 +2203,6 @@
     <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2037,65 +2215,47 @@
     <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="17" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="24" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="24" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="23" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="23" borderId="13" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="23" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="23" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="24" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="17" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="23" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="23" fillId="23" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="20% - Accent5" xfId="5" builtinId="46"/>
     <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
     <cellStyle name="Accent5" xfId="4" builtinId="45"/>
@@ -2104,6 +2264,7 @@
     <cellStyle name="Ieșire" xfId="3" builtinId="21"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notă" xfId="2" builtinId="10"/>
+    <cellStyle name="Virgulă" xfId="8" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3043,10 +3204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W75"/>
+  <dimension ref="A1:W153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,11 +3218,11 @@
     <col min="4" max="4" width="13.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" style="11" customWidth="1"/>
     <col min="6" max="6" width="22" style="11" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="45.85546875" style="11" customWidth="1"/>
     <col min="8" max="8" width="20" style="11" customWidth="1"/>
     <col min="9" max="9" width="24.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="23" style="11" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="11" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" style="11" customWidth="1"/>
     <col min="13" max="13" width="18.7109375" style="11" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" style="11" customWidth="1"/>
@@ -3084,23 +3245,23 @@
       <c r="B1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="94" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="90" t="s">
+      <c r="G1" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -3109,15 +3270,15 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="91"/>
+      <c r="C2" s="95"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
-      <c r="I2" s="91"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
@@ -3369,30 +3530,30 @@
       <c r="V15" s="15"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="84" t="s">
+      <c r="A16" s="102" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="84"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="84"/>
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
-      <c r="T16" s="84"/>
-      <c r="U16" s="84"/>
-      <c r="V16" s="84"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
+      <c r="P16" s="102"/>
+      <c r="Q16" s="102"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="102"/>
+      <c r="T16" s="102"/>
+      <c r="U16" s="102"/>
+      <c r="V16" s="102"/>
     </row>
     <row r="17" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
@@ -3400,18 +3561,18 @@
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="83" t="s">
+      <c r="F17" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="83"/>
-      <c r="H17" s="83"/>
-      <c r="I17" s="83"/>
-      <c r="J17" s="83" t="s">
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="96"/>
+      <c r="J17" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="K17" s="83"/>
-      <c r="L17" s="83"/>
-      <c r="M17" s="83"/>
+      <c r="K17" s="96"/>
+      <c r="L17" s="96"/>
+      <c r="M17" s="96"/>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -3453,10 +3614,10 @@
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="15"/>
-      <c r="O18" s="86" t="s">
+      <c r="O18" s="104" t="s">
         <v>91</v>
       </c>
-      <c r="P18" s="86"/>
+      <c r="P18" s="104"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
@@ -3895,12 +4056,12 @@
       <c r="V28" s="15"/>
     </row>
     <row r="29" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="92" t="s">
+      <c r="A29" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="92"/>
-      <c r="C29" s="92"/>
-      <c r="D29" s="92"/>
+      <c r="B29" s="97"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="97"/>
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
       <c r="G29" s="29" t="s">
@@ -4130,26 +4291,26 @@
       <c r="V34" s="15"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="85" t="s">
+      <c r="A37" s="103" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="85"/>
-      <c r="C37" s="85"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="85"/>
-      <c r="J37" s="85"/>
-      <c r="K37" s="85"/>
-      <c r="L37" s="85"/>
-      <c r="M37" s="85"/>
-      <c r="N37" s="85"/>
-      <c r="O37" s="85"/>
-      <c r="P37" s="85"/>
-      <c r="Q37" s="85"/>
-      <c r="R37" s="85"/>
+      <c r="B37" s="103"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="103"/>
+      <c r="F37" s="103"/>
+      <c r="G37" s="103"/>
+      <c r="H37" s="103"/>
+      <c r="I37" s="103"/>
+      <c r="J37" s="103"/>
+      <c r="K37" s="103"/>
+      <c r="L37" s="103"/>
+      <c r="M37" s="103"/>
+      <c r="N37" s="103"/>
+      <c r="O37" s="103"/>
+      <c r="P37" s="103"/>
+      <c r="Q37" s="103"/>
+      <c r="R37" s="103"/>
       <c r="S37" s="39"/>
       <c r="T37" s="39"/>
       <c r="U37" s="39"/>
@@ -4166,25 +4327,25 @@
       <c r="D38" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="82" t="s">
+      <c r="E38" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="82" t="s">
+      <c r="F38" s="101"/>
+      <c r="G38" s="101"/>
+      <c r="H38" s="101"/>
+      <c r="I38" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="J38" s="82"/>
-      <c r="K38" s="82"/>
-      <c r="L38" s="82"/>
-      <c r="M38" s="87" t="s">
+      <c r="J38" s="101"/>
+      <c r="K38" s="101"/>
+      <c r="L38" s="101"/>
+      <c r="M38" s="105" t="s">
         <v>91</v>
       </c>
-      <c r="N38" s="87"/>
-      <c r="O38" s="87"/>
-      <c r="P38" s="87"/>
-      <c r="Q38" s="87"/>
+      <c r="N38" s="105"/>
+      <c r="O38" s="105"/>
+      <c r="P38" s="105"/>
+      <c r="Q38" s="105"/>
       <c r="R38" s="39"/>
       <c r="S38" s="39"/>
       <c r="T38" s="39"/>
@@ -4865,120 +5026,120 @@
       <c r="V54" s="39"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A55" s="100" t="s">
+      <c r="A55" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="100"/>
-      <c r="C55" s="100"/>
-      <c r="D55" s="100"/>
-      <c r="E55" s="100"/>
-      <c r="F55" s="100"/>
-      <c r="G55" s="100"/>
-      <c r="H55" s="100"/>
-      <c r="I55" s="100"/>
-      <c r="J55" s="100"/>
-      <c r="K55" s="100"/>
-      <c r="L55" s="100"/>
-      <c r="M55" s="100"/>
-      <c r="N55" s="100"/>
-      <c r="O55" s="100"/>
-      <c r="P55" s="100"/>
-      <c r="Q55" s="100"/>
-      <c r="R55" s="100"/>
-      <c r="S55" s="100"/>
-      <c r="T55" s="89" t="s">
+      <c r="B55" s="88"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="88"/>
+      <c r="F55" s="88"/>
+      <c r="G55" s="88"/>
+      <c r="H55" s="88"/>
+      <c r="I55" s="88"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="88"/>
+      <c r="L55" s="88"/>
+      <c r="M55" s="88"/>
+      <c r="N55" s="88"/>
+      <c r="O55" s="88"/>
+      <c r="P55" s="88"/>
+      <c r="Q55" s="88"/>
+      <c r="R55" s="88"/>
+      <c r="S55" s="88"/>
+      <c r="T55" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="U55" s="89"/>
-      <c r="V55" s="89"/>
-      <c r="W55" s="105"/>
+      <c r="U55" s="106"/>
+      <c r="V55" s="106"/>
+      <c r="W55" s="82"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A56" s="100"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="100"/>
-      <c r="D56" s="100"/>
-      <c r="E56" s="100"/>
-      <c r="F56" s="100"/>
-      <c r="G56" s="100"/>
-      <c r="H56" s="100"/>
-      <c r="I56" s="100"/>
-      <c r="J56" s="100"/>
-      <c r="K56" s="100"/>
-      <c r="L56" s="100"/>
-      <c r="M56" s="100"/>
-      <c r="N56" s="100"/>
-      <c r="O56" s="100"/>
-      <c r="P56" s="100"/>
-      <c r="Q56" s="100"/>
-      <c r="R56" s="100"/>
-      <c r="S56" s="100"/>
-      <c r="T56" s="89"/>
-      <c r="U56" s="89"/>
-      <c r="V56" s="89"/>
-      <c r="W56" s="105"/>
+      <c r="A56" s="88"/>
+      <c r="B56" s="88"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="88"/>
+      <c r="F56" s="88"/>
+      <c r="G56" s="88"/>
+      <c r="H56" s="88"/>
+      <c r="I56" s="88"/>
+      <c r="J56" s="88"/>
+      <c r="K56" s="88"/>
+      <c r="L56" s="88"/>
+      <c r="M56" s="88"/>
+      <c r="N56" s="88"/>
+      <c r="O56" s="88"/>
+      <c r="P56" s="88"/>
+      <c r="Q56" s="88"/>
+      <c r="R56" s="88"/>
+      <c r="S56" s="88"/>
+      <c r="T56" s="106"/>
+      <c r="U56" s="106"/>
+      <c r="V56" s="106"/>
+      <c r="W56" s="82"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A57" s="82" t="s">
+      <c r="A57" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="82"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="88" t="s">
+      <c r="B57" s="101"/>
+      <c r="C57" s="101"/>
+      <c r="D57" s="89" t="s">
         <v>125</v>
       </c>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88" t="s">
+      <c r="E57" s="89"/>
+      <c r="F57" s="89" t="s">
         <v>127</v>
       </c>
-      <c r="G57" s="88"/>
-      <c r="H57" s="88" t="s">
+      <c r="G57" s="89"/>
+      <c r="H57" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="I57" s="88"/>
-      <c r="J57" s="88" t="s">
+      <c r="I57" s="89"/>
+      <c r="J57" s="89" t="s">
         <v>129</v>
       </c>
-      <c r="K57" s="88"/>
-      <c r="L57" s="88"/>
-      <c r="M57" s="88"/>
-      <c r="N57" s="88"/>
-      <c r="O57" s="88"/>
-      <c r="P57" s="88" t="s">
+      <c r="K57" s="89"/>
+      <c r="L57" s="89"/>
+      <c r="M57" s="89"/>
+      <c r="N57" s="89"/>
+      <c r="O57" s="89"/>
+      <c r="P57" s="89" t="s">
         <v>126</v>
       </c>
-      <c r="Q57" s="88"/>
-      <c r="R57" s="88"/>
-      <c r="S57" s="101"/>
-      <c r="T57" s="89"/>
-      <c r="U57" s="89"/>
-      <c r="V57" s="89"/>
-      <c r="W57" s="105"/>
+      <c r="Q57" s="89"/>
+      <c r="R57" s="89"/>
+      <c r="S57" s="90"/>
+      <c r="T57" s="106"/>
+      <c r="U57" s="106"/>
+      <c r="V57" s="106"/>
+      <c r="W57" s="82"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A58" s="82"/>
-      <c r="B58" s="82"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="88"/>
-      <c r="G58" s="88"/>
-      <c r="H58" s="88"/>
-      <c r="I58" s="88"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="88"/>
-      <c r="L58" s="88"/>
-      <c r="M58" s="88"/>
-      <c r="N58" s="88"/>
-      <c r="O58" s="88"/>
-      <c r="P58" s="88"/>
-      <c r="Q58" s="88"/>
-      <c r="R58" s="88"/>
-      <c r="S58" s="101"/>
-      <c r="T58" s="89"/>
-      <c r="U58" s="89"/>
-      <c r="V58" s="89"/>
-      <c r="W58" s="105"/>
+      <c r="A58" s="101"/>
+      <c r="B58" s="101"/>
+      <c r="C58" s="101"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="89"/>
+      <c r="G58" s="89"/>
+      <c r="H58" s="89"/>
+      <c r="I58" s="89"/>
+      <c r="J58" s="89"/>
+      <c r="K58" s="89"/>
+      <c r="L58" s="89"/>
+      <c r="M58" s="89"/>
+      <c r="N58" s="89"/>
+      <c r="O58" s="89"/>
+      <c r="P58" s="89"/>
+      <c r="Q58" s="89"/>
+      <c r="R58" s="89"/>
+      <c r="S58" s="90"/>
+      <c r="T58" s="106"/>
+      <c r="U58" s="106"/>
+      <c r="V58" s="106"/>
+      <c r="W58" s="82"/>
     </row>
     <row r="59" spans="1:23" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="69" t="s">
@@ -4990,39 +5151,39 @@
       <c r="C59" s="71">
         <v>20.646896487046401</v>
       </c>
-      <c r="D59" s="93">
+      <c r="D59" s="84">
         <v>16</v>
       </c>
-      <c r="E59" s="93"/>
-      <c r="F59" s="93">
+      <c r="E59" s="84"/>
+      <c r="F59" s="84">
         <v>62</v>
       </c>
-      <c r="G59" s="93"/>
-      <c r="H59" s="93">
+      <c r="G59" s="84"/>
+      <c r="H59" s="84">
         <f>F59/D59</f>
         <v>3.875</v>
       </c>
-      <c r="I59" s="93"/>
-      <c r="J59" s="93">
+      <c r="I59" s="84"/>
+      <c r="J59" s="84">
         <f>((G7-H59)/C39)*100</f>
         <v>0</v>
       </c>
-      <c r="K59" s="93"/>
-      <c r="L59" s="93"/>
-      <c r="M59" s="93"/>
-      <c r="N59" s="93"/>
-      <c r="O59" s="93"/>
-      <c r="P59" s="93">
+      <c r="K59" s="84"/>
+      <c r="L59" s="84"/>
+      <c r="M59" s="84"/>
+      <c r="N59" s="84"/>
+      <c r="O59" s="84"/>
+      <c r="P59" s="84">
         <v>222.0667</v>
       </c>
-      <c r="Q59" s="93"/>
-      <c r="R59" s="93"/>
-      <c r="S59" s="102"/>
-      <c r="T59" s="93" t="s">
+      <c r="Q59" s="84"/>
+      <c r="R59" s="84"/>
+      <c r="S59" s="91"/>
+      <c r="T59" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="U59" s="93"/>
-      <c r="V59" s="93"/>
+      <c r="U59" s="84"/>
+      <c r="V59" s="84"/>
     </row>
     <row r="60" spans="1:23" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="69" t="s">
@@ -5034,40 +5195,40 @@
       <c r="C60" s="72">
         <v>22.546048321514299</v>
       </c>
-      <c r="D60" s="94">
+      <c r="D60" s="92">
         <v>16</v>
       </c>
-      <c r="E60" s="94"/>
-      <c r="F60" s="94">
+      <c r="E60" s="92"/>
+      <c r="F60" s="92">
         <v>63</v>
       </c>
-      <c r="G60" s="94"/>
-      <c r="H60" s="94">
+      <c r="G60" s="92"/>
+      <c r="H60" s="92">
         <f>F60/D60</f>
         <v>3.9375</v>
       </c>
-      <c r="I60" s="94"/>
-      <c r="J60" s="94">
+      <c r="I60" s="92"/>
+      <c r="J60" s="92">
         <f>((G7-H60)/C$39)*100</f>
         <v>-1.6129032258064515</v>
       </c>
-      <c r="K60" s="94"/>
-      <c r="L60" s="94"/>
-      <c r="M60" s="94"/>
-      <c r="N60" s="94"/>
-      <c r="O60" s="94"/>
-      <c r="P60" s="94">
+      <c r="K60" s="92"/>
+      <c r="L60" s="92"/>
+      <c r="M60" s="92"/>
+      <c r="N60" s="92"/>
+      <c r="O60" s="92"/>
+      <c r="P60" s="92">
         <v>224.91374999999999</v>
       </c>
-      <c r="Q60" s="94"/>
-      <c r="R60" s="94"/>
-      <c r="S60" s="103"/>
-      <c r="T60" s="106" t="b">
+      <c r="Q60" s="92"/>
+      <c r="R60" s="92"/>
+      <c r="S60" s="93"/>
+      <c r="T60" s="85" t="b">
         <f>-2.75&lt;0.08625&lt;5.5</f>
         <v>0</v>
       </c>
-      <c r="U60" s="106"/>
-      <c r="V60" s="106"/>
+      <c r="U60" s="85"/>
+      <c r="V60" s="85"/>
       <c r="W60" s="39">
         <f>225-P60</f>
         <v>8.6250000000006821E-2</v>
@@ -5083,40 +5244,40 @@
       <c r="C61" s="72">
         <v>0.55711257339562903</v>
       </c>
-      <c r="D61" s="95">
+      <c r="D61" s="86">
         <v>17</v>
       </c>
-      <c r="E61" s="95"/>
-      <c r="F61" s="95">
+      <c r="E61" s="86"/>
+      <c r="F61" s="86">
         <v>62</v>
       </c>
-      <c r="G61" s="95"/>
-      <c r="H61" s="95">
+      <c r="G61" s="86"/>
+      <c r="H61" s="86">
         <f>F61/D61</f>
         <v>3.6470588235294117</v>
       </c>
-      <c r="I61" s="95"/>
-      <c r="J61" s="95">
+      <c r="I61" s="86"/>
+      <c r="J61" s="86">
         <f>((G7-H61)/G7)*100</f>
         <v>5.8823529411764728</v>
       </c>
-      <c r="K61" s="95"/>
-      <c r="L61" s="95"/>
-      <c r="M61" s="95"/>
-      <c r="N61" s="95"/>
-      <c r="O61" s="95"/>
-      <c r="P61" s="95">
+      <c r="K61" s="86"/>
+      <c r="L61" s="86"/>
+      <c r="M61" s="86"/>
+      <c r="N61" s="86"/>
+      <c r="O61" s="86"/>
+      <c r="P61" s="86">
         <v>224.91374999999999</v>
       </c>
-      <c r="Q61" s="95"/>
-      <c r="R61" s="95"/>
-      <c r="S61" s="99"/>
-      <c r="T61" s="106" t="b">
+      <c r="Q61" s="86"/>
+      <c r="R61" s="86"/>
+      <c r="S61" s="87"/>
+      <c r="T61" s="85" t="b">
         <f>-0.5*5.5&lt;225-P61&lt;=5.5</f>
         <v>0</v>
       </c>
-      <c r="U61" s="106"/>
-      <c r="V61" s="106"/>
+      <c r="U61" s="85"/>
+      <c r="V61" s="85"/>
     </row>
     <row r="62" spans="1:23" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="69" t="s">
@@ -5128,40 +5289,40 @@
       <c r="C62" s="72">
         <v>0.410419384902517</v>
       </c>
-      <c r="D62" s="95">
+      <c r="D62" s="86">
         <v>17</v>
       </c>
-      <c r="E62" s="95"/>
-      <c r="F62" s="95">
+      <c r="E62" s="86"/>
+      <c r="F62" s="86">
         <v>63</v>
       </c>
-      <c r="G62" s="95"/>
-      <c r="H62" s="95">
+      <c r="G62" s="86"/>
+      <c r="H62" s="86">
         <f>F62/D62</f>
         <v>3.7058823529411766</v>
       </c>
-      <c r="I62" s="95"/>
-      <c r="J62" s="95">
+      <c r="I62" s="86"/>
+      <c r="J62" s="86">
         <f>((G7-H62)/C39)*100</f>
         <v>4.3643263757115713</v>
       </c>
-      <c r="K62" s="95"/>
-      <c r="L62" s="95"/>
-      <c r="M62" s="95"/>
-      <c r="N62" s="95"/>
-      <c r="O62" s="95"/>
-      <c r="P62" s="95">
+      <c r="K62" s="86"/>
+      <c r="L62" s="86"/>
+      <c r="M62" s="86"/>
+      <c r="N62" s="86"/>
+      <c r="O62" s="86"/>
+      <c r="P62" s="86">
         <v>227.76075968999999</v>
       </c>
-      <c r="Q62" s="95"/>
-      <c r="R62" s="95"/>
-      <c r="S62" s="99"/>
-      <c r="T62" s="106" t="b">
+      <c r="Q62" s="86"/>
+      <c r="R62" s="86"/>
+      <c r="S62" s="87"/>
+      <c r="T62" s="85" t="b">
         <f>-0.5*5.5&lt;225-P62&lt;=5.5</f>
         <v>0</v>
       </c>
-      <c r="U62" s="106"/>
-      <c r="V62" s="106"/>
+      <c r="U62" s="85"/>
+      <c r="V62" s="85"/>
     </row>
     <row r="63" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="74"/>
@@ -5195,124 +5356,124 @@
       <c r="C64" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="104"/>
-      <c r="E64" s="104"/>
-      <c r="F64" s="104"/>
-      <c r="G64" s="104"/>
-      <c r="H64" s="104"/>
-      <c r="I64" s="104"/>
-      <c r="J64" s="104"/>
-      <c r="K64" s="104"/>
-      <c r="L64" s="104"/>
-      <c r="M64" s="104"/>
-      <c r="N64" s="104"/>
-      <c r="O64" s="104"/>
-      <c r="P64" s="104"/>
-      <c r="Q64" s="104"/>
-      <c r="R64" s="104"/>
+      <c r="D64" s="83"/>
+      <c r="E64" s="83"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="83"/>
+      <c r="H64" s="83"/>
+      <c r="I64" s="83"/>
+      <c r="J64" s="83"/>
+      <c r="K64" s="83"/>
+      <c r="L64" s="83"/>
+      <c r="M64" s="83"/>
+      <c r="N64" s="83"/>
+      <c r="O64" s="83"/>
+      <c r="P64" s="83"/>
+      <c r="Q64" s="83"/>
+      <c r="R64" s="83"/>
       <c r="S64" s="64"/>
-      <c r="T64" s="96"/>
-      <c r="U64" s="97"/>
-      <c r="V64" s="98"/>
+      <c r="T64" s="79"/>
+      <c r="U64" s="80"/>
+      <c r="V64" s="81"/>
     </row>
     <row r="65" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
-      <c r="D65" s="104"/>
-      <c r="E65" s="104"/>
-      <c r="F65" s="104"/>
-      <c r="G65" s="104"/>
-      <c r="H65" s="104"/>
-      <c r="I65" s="104"/>
-      <c r="J65" s="104"/>
-      <c r="K65" s="104"/>
-      <c r="L65" s="104"/>
-      <c r="M65" s="104"/>
-      <c r="N65" s="104"/>
-      <c r="O65" s="104"/>
-      <c r="P65" s="104"/>
-      <c r="Q65" s="104"/>
-      <c r="R65" s="104"/>
+      <c r="D65" s="83"/>
+      <c r="E65" s="83"/>
+      <c r="F65" s="83"/>
+      <c r="G65" s="83"/>
+      <c r="H65" s="83"/>
+      <c r="I65" s="83"/>
+      <c r="J65" s="83"/>
+      <c r="K65" s="83"/>
+      <c r="L65" s="83"/>
+      <c r="M65" s="83"/>
+      <c r="N65" s="83"/>
+      <c r="O65" s="83"/>
+      <c r="P65" s="83"/>
+      <c r="Q65" s="83"/>
+      <c r="R65" s="83"/>
       <c r="S65" s="64"/>
-      <c r="T65" s="96"/>
-      <c r="U65" s="97"/>
-      <c r="V65" s="98"/>
+      <c r="T65" s="79"/>
+      <c r="U65" s="80"/>
+      <c r="V65" s="81"/>
     </row>
     <row r="66" spans="1:22" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
-      <c r="D66" s="104"/>
-      <c r="E66" s="104"/>
-      <c r="F66" s="104"/>
-      <c r="G66" s="104"/>
-      <c r="H66" s="104"/>
-      <c r="I66" s="104"/>
-      <c r="J66" s="104"/>
-      <c r="K66" s="104"/>
-      <c r="L66" s="104"/>
-      <c r="M66" s="104"/>
-      <c r="N66" s="104"/>
-      <c r="O66" s="104"/>
-      <c r="P66" s="104"/>
-      <c r="Q66" s="104"/>
-      <c r="R66" s="104"/>
+      <c r="D66" s="83"/>
+      <c r="E66" s="83"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="83"/>
+      <c r="H66" s="83"/>
+      <c r="I66" s="83"/>
+      <c r="J66" s="83"/>
+      <c r="K66" s="83"/>
+      <c r="L66" s="83"/>
+      <c r="M66" s="83"/>
+      <c r="N66" s="83"/>
+      <c r="O66" s="83"/>
+      <c r="P66" s="83"/>
+      <c r="Q66" s="83"/>
+      <c r="R66" s="83"/>
       <c r="S66" s="64"/>
-      <c r="T66" s="96"/>
-      <c r="U66" s="97"/>
-      <c r="V66" s="98"/>
+      <c r="T66" s="79"/>
+      <c r="U66" s="80"/>
+      <c r="V66" s="81"/>
     </row>
     <row r="67" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
-      <c r="D67" s="104"/>
-      <c r="E67" s="104"/>
-      <c r="F67" s="104"/>
-      <c r="G67" s="104"/>
-      <c r="H67" s="104"/>
-      <c r="I67" s="104"/>
-      <c r="J67" s="104"/>
-      <c r="K67" s="104"/>
-      <c r="L67" s="104"/>
-      <c r="M67" s="104"/>
-      <c r="N67" s="104"/>
-      <c r="O67" s="104"/>
-      <c r="P67" s="104"/>
-      <c r="Q67" s="104"/>
-      <c r="R67" s="104"/>
+      <c r="D67" s="83"/>
+      <c r="E67" s="83"/>
+      <c r="F67" s="83"/>
+      <c r="G67" s="83"/>
+      <c r="H67" s="83"/>
+      <c r="I67" s="83"/>
+      <c r="J67" s="83"/>
+      <c r="K67" s="83"/>
+      <c r="L67" s="83"/>
+      <c r="M67" s="83"/>
+      <c r="N67" s="83"/>
+      <c r="O67" s="83"/>
+      <c r="P67" s="83"/>
+      <c r="Q67" s="83"/>
+      <c r="R67" s="83"/>
       <c r="S67" s="64"/>
-      <c r="T67" s="96"/>
-      <c r="U67" s="97"/>
-      <c r="V67" s="98"/>
+      <c r="T67" s="79"/>
+      <c r="U67" s="80"/>
+      <c r="V67" s="81"/>
     </row>
     <row r="71" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="80" t="s">
+      <c r="B71" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="81"/>
-      <c r="D71" s="79" t="s">
+      <c r="C71" s="100"/>
+      <c r="D71" s="98" t="s">
         <v>137</v>
       </c>
-      <c r="E71" s="79"/>
-      <c r="F71" s="79"/>
-      <c r="G71" s="79"/>
-      <c r="H71" s="79"/>
-      <c r="I71" s="79"/>
-      <c r="J71" s="79"/>
-      <c r="K71" s="79"/>
-      <c r="L71" s="79"/>
-      <c r="M71" s="79"/>
-      <c r="N71" s="79"/>
-      <c r="O71" s="79"/>
-      <c r="P71" s="79"/>
-      <c r="Q71" s="79"/>
-      <c r="R71" s="79"/>
+      <c r="E71" s="98"/>
+      <c r="F71" s="98"/>
+      <c r="G71" s="98"/>
+      <c r="H71" s="98"/>
+      <c r="I71" s="98"/>
+      <c r="J71" s="98"/>
+      <c r="K71" s="98"/>
+      <c r="L71" s="98"/>
+      <c r="M71" s="98"/>
+      <c r="N71" s="98"/>
+      <c r="O71" s="98"/>
+      <c r="P71" s="98"/>
+      <c r="Q71" s="98"/>
+      <c r="R71" s="98"/>
     </row>
     <row r="72" spans="1:22" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="80"/>
-      <c r="C72" s="81"/>
+      <c r="B72" s="99"/>
+      <c r="C72" s="100"/>
       <c r="D72" s="78" t="s">
         <v>139</v>
       </c>
@@ -5350,8 +5511,8 @@
       <c r="R72" s="78"/>
     </row>
     <row r="73" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="80"/>
-      <c r="C73" s="81"/>
+      <c r="B73" s="99"/>
+      <c r="C73" s="100"/>
       <c r="D73" s="78" t="s">
         <v>149</v>
       </c>
@@ -5374,8 +5535,8 @@
       <c r="R73" s="78"/>
     </row>
     <row r="74" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="80"/>
-      <c r="C74" s="81"/>
+      <c r="B74" s="99"/>
+      <c r="C74" s="100"/>
       <c r="D74" s="78" t="s">
         <v>150</v>
       </c>
@@ -5398,8 +5559,8 @@
       <c r="R74" s="78"/>
     </row>
     <row r="75" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="80"/>
-      <c r="C75" s="81"/>
+      <c r="B75" s="99"/>
+      <c r="C75" s="100"/>
       <c r="D75" s="78" t="s">
         <v>151</v>
       </c>
@@ -5418,8 +5579,1575 @@
       <c r="Q75" s="78"/>
       <c r="R75" s="78"/>
     </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B77" s="107"/>
+      <c r="C77" s="107"/>
+      <c r="D77" s="107"/>
+      <c r="E77" s="107"/>
+      <c r="F77" s="107"/>
+      <c r="G77" s="107"/>
+      <c r="H77" s="107"/>
+      <c r="I77" s="107"/>
+      <c r="J77" s="107"/>
+      <c r="K77" s="107"/>
+      <c r="L77" s="107"/>
+      <c r="M77" s="107"/>
+      <c r="N77" s="107"/>
+      <c r="O77" s="107"/>
+      <c r="P77" s="107"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B78" s="107"/>
+      <c r="C78" s="107"/>
+      <c r="D78" s="107"/>
+      <c r="E78" s="109"/>
+      <c r="F78" s="109"/>
+      <c r="G78" s="109"/>
+      <c r="H78" s="107"/>
+      <c r="I78" s="107"/>
+      <c r="J78" s="107"/>
+      <c r="K78" s="107"/>
+      <c r="L78" s="107"/>
+      <c r="M78" s="107"/>
+      <c r="N78" s="107"/>
+      <c r="O78" s="107"/>
+      <c r="P78" s="107"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B79" s="107"/>
+      <c r="C79" s="107"/>
+      <c r="D79" s="107"/>
+      <c r="E79" s="112" t="s">
+        <v>152</v>
+      </c>
+      <c r="F79" s="112"/>
+      <c r="G79" s="115"/>
+      <c r="H79" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="I79" s="112"/>
+      <c r="J79" s="112"/>
+      <c r="K79" s="113" t="s">
+        <v>173</v>
+      </c>
+      <c r="L79" s="114"/>
+      <c r="M79" s="114"/>
+      <c r="N79" s="108"/>
+      <c r="O79" s="108"/>
+      <c r="P79" s="108"/>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B80" s="107"/>
+      <c r="C80" s="107"/>
+      <c r="D80" s="107"/>
+      <c r="E80" s="112"/>
+      <c r="F80" s="112"/>
+      <c r="G80" s="115"/>
+      <c r="H80" s="112"/>
+      <c r="I80" s="112"/>
+      <c r="J80" s="112"/>
+      <c r="K80" s="113"/>
+      <c r="L80" s="114"/>
+      <c r="M80" s="114"/>
+      <c r="N80" s="108"/>
+      <c r="O80" s="108"/>
+      <c r="P80" s="108"/>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B81" s="107"/>
+      <c r="C81" s="107"/>
+      <c r="D81" s="107"/>
+      <c r="E81" s="112"/>
+      <c r="F81" s="112"/>
+      <c r="G81" s="115"/>
+      <c r="H81" s="112"/>
+      <c r="I81" s="112"/>
+      <c r="J81" s="112"/>
+      <c r="K81" s="113"/>
+      <c r="L81" s="114"/>
+      <c r="M81" s="114"/>
+      <c r="N81" s="108"/>
+      <c r="O81" s="108"/>
+      <c r="P81" s="108"/>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B82" s="107"/>
+      <c r="C82" s="107"/>
+      <c r="D82" s="107"/>
+      <c r="E82" s="112"/>
+      <c r="F82" s="112"/>
+      <c r="G82" s="115"/>
+      <c r="H82" s="112"/>
+      <c r="I82" s="112"/>
+      <c r="J82" s="112"/>
+      <c r="K82" s="117"/>
+      <c r="L82" s="118"/>
+      <c r="M82" s="118"/>
+      <c r="N82" s="108"/>
+      <c r="O82" s="108"/>
+      <c r="P82" s="108"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B83" s="107"/>
+      <c r="C83" s="107"/>
+      <c r="D83" s="107"/>
+      <c r="E83" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="F83" s="110">
+        <v>17</v>
+      </c>
+      <c r="G83" s="116"/>
+      <c r="H83" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="I83" s="110"/>
+      <c r="J83" s="110"/>
+      <c r="K83" s="110" t="s">
+        <v>125</v>
+      </c>
+      <c r="L83" s="110"/>
+      <c r="M83" s="110"/>
+      <c r="N83" s="107"/>
+      <c r="O83" s="107"/>
+      <c r="P83" s="107"/>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B84" s="107"/>
+      <c r="C84" s="107"/>
+      <c r="D84" s="107"/>
+      <c r="E84" s="110" t="s">
+        <v>127</v>
+      </c>
+      <c r="F84" s="110">
+        <v>78</v>
+      </c>
+      <c r="G84" s="116"/>
+      <c r="H84" s="110" t="s">
+        <v>127</v>
+      </c>
+      <c r="I84" s="110"/>
+      <c r="J84" s="110"/>
+      <c r="K84" s="110" t="s">
+        <v>127</v>
+      </c>
+      <c r="L84" s="110"/>
+      <c r="M84" s="110"/>
+      <c r="N84" s="107"/>
+      <c r="O84" s="107"/>
+      <c r="P84" s="107"/>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B85" s="107"/>
+      <c r="C85" s="107"/>
+      <c r="D85" s="107"/>
+      <c r="E85" s="110" t="s">
+        <v>154</v>
+      </c>
+      <c r="F85" s="110">
+        <v>4</v>
+      </c>
+      <c r="G85" s="116"/>
+      <c r="H85" s="110" t="s">
+        <v>154</v>
+      </c>
+      <c r="I85" s="110"/>
+      <c r="J85" s="110"/>
+      <c r="K85" s="110" t="s">
+        <v>154</v>
+      </c>
+      <c r="L85" s="110"/>
+      <c r="M85" s="110"/>
+      <c r="N85" s="107"/>
+      <c r="O85" s="107"/>
+      <c r="P85" s="107"/>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B86" s="107"/>
+      <c r="C86" s="107"/>
+      <c r="D86" s="107"/>
+      <c r="E86" s="110" t="s">
+        <v>155</v>
+      </c>
+      <c r="F86" s="110">
+        <v>35</v>
+      </c>
+      <c r="G86" s="116"/>
+      <c r="H86" s="110" t="s">
+        <v>155</v>
+      </c>
+      <c r="I86" s="110"/>
+      <c r="J86" s="110"/>
+      <c r="K86" s="110" t="s">
+        <v>155</v>
+      </c>
+      <c r="L86" s="110"/>
+      <c r="M86" s="110"/>
+      <c r="N86" s="107"/>
+      <c r="O86" s="107"/>
+      <c r="P86" s="107"/>
+    </row>
+    <row r="87" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B87" s="107"/>
+      <c r="C87" s="107"/>
+      <c r="D87" s="107"/>
+      <c r="E87" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="F87" s="110">
+        <v>4.5</v>
+      </c>
+      <c r="G87" s="116"/>
+      <c r="H87" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="I87" s="110"/>
+      <c r="J87" s="110"/>
+      <c r="K87" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="L87" s="110"/>
+      <c r="M87" s="110"/>
+      <c r="N87" s="107"/>
+      <c r="O87" s="107"/>
+      <c r="P87" s="107"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B88" s="107"/>
+      <c r="C88" s="107"/>
+      <c r="D88" s="107"/>
+      <c r="E88" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="F88" s="110">
+        <v>38.25</v>
+      </c>
+      <c r="G88" s="116"/>
+      <c r="H88" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="I88" s="110"/>
+      <c r="J88" s="110"/>
+      <c r="K88" s="110" t="s">
+        <v>82</v>
+      </c>
+      <c r="L88" s="110"/>
+      <c r="M88" s="110"/>
+      <c r="N88" s="107"/>
+      <c r="O88" s="107"/>
+      <c r="P88" s="107"/>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B89" s="107"/>
+      <c r="C89" s="107"/>
+      <c r="D89" s="107"/>
+      <c r="E89" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="F89" s="110">
+        <v>58</v>
+      </c>
+      <c r="G89" s="116"/>
+      <c r="H89" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="I89" s="110"/>
+      <c r="J89" s="110"/>
+      <c r="K89" s="110" t="s">
+        <v>157</v>
+      </c>
+      <c r="L89" s="110"/>
+      <c r="M89" s="110"/>
+      <c r="N89" s="107"/>
+      <c r="O89" s="107"/>
+      <c r="P89" s="107"/>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B90" s="107"/>
+      <c r="C90" s="107"/>
+      <c r="D90" s="107"/>
+      <c r="E90" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="F90" s="110"/>
+      <c r="G90" s="116"/>
+      <c r="H90" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="I90" s="110"/>
+      <c r="J90" s="110"/>
+      <c r="K90" s="110" t="s">
+        <v>158</v>
+      </c>
+      <c r="L90" s="110"/>
+      <c r="M90" s="110"/>
+      <c r="N90" s="107"/>
+      <c r="O90" s="107"/>
+      <c r="P90" s="107"/>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B91" s="107"/>
+      <c r="C91" s="107"/>
+      <c r="D91" s="107"/>
+      <c r="E91" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="F91" s="110"/>
+      <c r="G91" s="116"/>
+      <c r="H91" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="I91" s="110"/>
+      <c r="J91" s="110"/>
+      <c r="K91" s="110" t="s">
+        <v>159</v>
+      </c>
+      <c r="L91" s="110"/>
+      <c r="M91" s="110"/>
+      <c r="N91" s="107"/>
+      <c r="O91" s="107"/>
+      <c r="P91" s="107"/>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B92" s="107"/>
+      <c r="C92" s="107"/>
+      <c r="D92" s="107"/>
+      <c r="E92" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="F92" s="110"/>
+      <c r="G92" s="116"/>
+      <c r="H92" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="I92" s="110"/>
+      <c r="J92" s="110"/>
+      <c r="K92" s="110" t="s">
+        <v>160</v>
+      </c>
+      <c r="L92" s="110"/>
+      <c r="M92" s="110"/>
+      <c r="N92" s="107"/>
+      <c r="O92" s="107"/>
+      <c r="P92" s="107"/>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B93" s="107"/>
+      <c r="C93" s="107"/>
+      <c r="D93" s="107"/>
+      <c r="E93" s="110" t="s">
+        <v>161</v>
+      </c>
+      <c r="F93" s="110"/>
+      <c r="G93" s="116"/>
+      <c r="H93" s="110" t="s">
+        <v>161</v>
+      </c>
+      <c r="I93" s="110"/>
+      <c r="J93" s="110"/>
+      <c r="K93" s="110" t="s">
+        <v>161</v>
+      </c>
+      <c r="L93" s="110"/>
+      <c r="M93" s="110"/>
+      <c r="N93" s="107"/>
+      <c r="O93" s="107"/>
+      <c r="P93" s="107"/>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B94" s="107"/>
+      <c r="C94" s="107"/>
+      <c r="D94" s="107"/>
+      <c r="E94" s="110" t="s">
+        <v>162</v>
+      </c>
+      <c r="F94" s="110"/>
+      <c r="G94" s="116"/>
+      <c r="H94" s="110" t="s">
+        <v>162</v>
+      </c>
+      <c r="I94" s="110"/>
+      <c r="J94" s="110"/>
+      <c r="K94" s="110" t="s">
+        <v>162</v>
+      </c>
+      <c r="L94" s="110"/>
+      <c r="M94" s="110"/>
+      <c r="N94" s="107"/>
+      <c r="O94" s="107"/>
+      <c r="P94" s="107"/>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B95" s="107"/>
+      <c r="C95" s="107"/>
+      <c r="D95" s="107"/>
+      <c r="E95" s="110" t="s">
+        <v>163</v>
+      </c>
+      <c r="F95" s="110"/>
+      <c r="G95" s="116"/>
+      <c r="H95" s="110" t="s">
+        <v>163</v>
+      </c>
+      <c r="I95" s="110"/>
+      <c r="J95" s="110"/>
+      <c r="K95" s="110" t="s">
+        <v>163</v>
+      </c>
+      <c r="L95" s="110"/>
+      <c r="M95" s="110"/>
+      <c r="N95" s="107"/>
+      <c r="O95" s="107"/>
+      <c r="P95" s="107"/>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B96" s="107"/>
+      <c r="C96" s="107"/>
+      <c r="D96" s="107"/>
+      <c r="E96" s="110" t="s">
+        <v>176</v>
+      </c>
+      <c r="F96" s="110">
+        <v>5</v>
+      </c>
+      <c r="G96" s="116"/>
+      <c r="H96" s="110" t="s">
+        <v>153</v>
+      </c>
+      <c r="I96" s="110"/>
+      <c r="J96" s="110"/>
+      <c r="K96" s="110" t="s">
+        <v>175</v>
+      </c>
+      <c r="L96" s="110">
+        <v>0</v>
+      </c>
+      <c r="M96" s="110"/>
+      <c r="N96" s="107"/>
+      <c r="O96" s="107"/>
+      <c r="P96" s="107"/>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B97" s="107"/>
+      <c r="C97" s="107"/>
+      <c r="D97" s="107"/>
+      <c r="E97" s="110" t="s">
+        <v>164</v>
+      </c>
+      <c r="F97" s="110"/>
+      <c r="G97" s="116"/>
+      <c r="H97" s="110" t="s">
+        <v>164</v>
+      </c>
+      <c r="I97" s="110"/>
+      <c r="J97" s="110"/>
+      <c r="K97" s="110" t="s">
+        <v>164</v>
+      </c>
+      <c r="L97" s="110"/>
+      <c r="M97" s="110"/>
+      <c r="N97" s="107"/>
+      <c r="O97" s="107"/>
+      <c r="P97" s="107"/>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B98" s="107"/>
+      <c r="C98" s="107"/>
+      <c r="D98" s="107"/>
+      <c r="E98" s="110" t="s">
+        <v>165</v>
+      </c>
+      <c r="F98" s="110">
+        <v>5</v>
+      </c>
+      <c r="G98" s="116"/>
+      <c r="H98" s="110" t="s">
+        <v>165</v>
+      </c>
+      <c r="I98" s="110"/>
+      <c r="J98" s="110"/>
+      <c r="K98" s="110" t="s">
+        <v>165</v>
+      </c>
+      <c r="L98" s="110"/>
+      <c r="M98" s="110"/>
+      <c r="N98" s="107"/>
+      <c r="O98" s="107"/>
+      <c r="P98" s="107"/>
+    </row>
+    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B99" s="107"/>
+      <c r="C99" s="107"/>
+      <c r="D99" s="107"/>
+      <c r="E99" s="110" t="s">
+        <v>166</v>
+      </c>
+      <c r="F99" s="110">
+        <v>38</v>
+      </c>
+      <c r="G99" s="116"/>
+      <c r="H99" s="110" t="s">
+        <v>166</v>
+      </c>
+      <c r="I99" s="110"/>
+      <c r="J99" s="110"/>
+      <c r="K99" s="110" t="s">
+        <v>166</v>
+      </c>
+      <c r="L99" s="110"/>
+      <c r="M99" s="110"/>
+      <c r="N99" s="107"/>
+      <c r="O99" s="107"/>
+      <c r="P99" s="107"/>
+    </row>
+    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B100" s="107"/>
+      <c r="C100" s="107"/>
+      <c r="D100" s="107"/>
+      <c r="E100" s="110" t="s">
+        <v>167</v>
+      </c>
+      <c r="F100" s="110"/>
+      <c r="G100" s="116"/>
+      <c r="H100" s="110" t="s">
+        <v>167</v>
+      </c>
+      <c r="I100" s="110"/>
+      <c r="J100" s="110"/>
+      <c r="K100" s="110" t="s">
+        <v>167</v>
+      </c>
+      <c r="L100" s="110"/>
+      <c r="M100" s="110"/>
+      <c r="N100" s="107"/>
+      <c r="O100" s="107"/>
+      <c r="P100" s="107"/>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B101" s="107"/>
+      <c r="C101" s="107"/>
+      <c r="D101" s="107"/>
+      <c r="E101" s="110" t="s">
+        <v>168</v>
+      </c>
+      <c r="F101" s="110"/>
+      <c r="G101" s="116"/>
+      <c r="H101" s="110" t="s">
+        <v>168</v>
+      </c>
+      <c r="I101" s="110"/>
+      <c r="J101" s="110"/>
+      <c r="K101" s="110" t="s">
+        <v>168</v>
+      </c>
+      <c r="L101" s="110"/>
+      <c r="M101" s="110"/>
+      <c r="N101" s="107"/>
+      <c r="O101" s="107"/>
+      <c r="P101" s="107"/>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B102" s="107"/>
+      <c r="C102" s="107"/>
+      <c r="D102" s="107"/>
+      <c r="E102" s="110" t="s">
+        <v>169</v>
+      </c>
+      <c r="F102" s="110"/>
+      <c r="G102" s="116"/>
+      <c r="H102" s="110" t="s">
+        <v>169</v>
+      </c>
+      <c r="I102" s="110"/>
+      <c r="J102" s="110"/>
+      <c r="K102" s="110" t="s">
+        <v>169</v>
+      </c>
+      <c r="L102" s="110"/>
+      <c r="M102" s="110"/>
+      <c r="N102" s="107"/>
+      <c r="O102" s="107"/>
+      <c r="P102" s="107"/>
+    </row>
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B103" s="107"/>
+      <c r="C103" s="107"/>
+      <c r="D103" s="107"/>
+      <c r="E103" s="110" t="s">
+        <v>170</v>
+      </c>
+      <c r="F103" s="110"/>
+      <c r="G103" s="116"/>
+      <c r="H103" s="110" t="s">
+        <v>170</v>
+      </c>
+      <c r="I103" s="110"/>
+      <c r="J103" s="110"/>
+      <c r="K103" s="110" t="s">
+        <v>170</v>
+      </c>
+      <c r="L103" s="110"/>
+      <c r="M103" s="110"/>
+      <c r="N103" s="107"/>
+      <c r="O103" s="107"/>
+      <c r="P103" s="107"/>
+    </row>
+    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B104" s="107"/>
+      <c r="C104" s="107"/>
+      <c r="D104" s="107"/>
+      <c r="E104" s="110" t="s">
+        <v>171</v>
+      </c>
+      <c r="F104" s="110"/>
+      <c r="G104" s="116"/>
+      <c r="H104" s="110" t="s">
+        <v>171</v>
+      </c>
+      <c r="I104" s="110"/>
+      <c r="J104" s="110"/>
+      <c r="K104" s="110" t="s">
+        <v>171</v>
+      </c>
+      <c r="L104" s="110"/>
+      <c r="M104" s="110"/>
+      <c r="N104" s="107"/>
+      <c r="O104" s="107"/>
+      <c r="P104" s="107"/>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B105" s="107"/>
+      <c r="C105" s="107"/>
+      <c r="D105" s="107"/>
+      <c r="E105" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="F105" s="110"/>
+      <c r="G105" s="116"/>
+      <c r="H105" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="I105" s="110"/>
+      <c r="J105" s="110"/>
+      <c r="K105" s="110" t="s">
+        <v>32</v>
+      </c>
+      <c r="L105" s="110"/>
+      <c r="M105" s="110"/>
+      <c r="N105" s="107"/>
+      <c r="O105" s="107"/>
+      <c r="P105" s="107"/>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B106" s="107"/>
+      <c r="C106" s="107"/>
+      <c r="D106" s="107"/>
+      <c r="E106" s="110" t="s">
+        <v>174</v>
+      </c>
+      <c r="F106" s="110">
+        <v>10</v>
+      </c>
+      <c r="G106" s="110"/>
+      <c r="H106" s="110" t="s">
+        <v>174</v>
+      </c>
+      <c r="I106" s="110"/>
+      <c r="J106" s="110"/>
+      <c r="K106" s="110" t="s">
+        <v>174</v>
+      </c>
+      <c r="L106" s="110"/>
+      <c r="M106" s="110"/>
+      <c r="N106" s="107"/>
+      <c r="O106" s="107"/>
+      <c r="P106" s="107"/>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B107" s="107"/>
+      <c r="C107" s="107"/>
+      <c r="D107" s="107"/>
+      <c r="E107" s="110" t="s">
+        <v>67</v>
+      </c>
+      <c r="F107" s="110">
+        <v>4</v>
+      </c>
+      <c r="G107" s="110"/>
+      <c r="H107" s="110"/>
+      <c r="I107" s="110"/>
+      <c r="J107" s="110"/>
+      <c r="K107" s="110"/>
+      <c r="L107" s="110"/>
+      <c r="M107" s="110"/>
+      <c r="N107" s="107"/>
+      <c r="O107" s="107"/>
+      <c r="P107" s="107"/>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B108" s="107"/>
+      <c r="C108" s="107"/>
+      <c r="D108" s="107"/>
+      <c r="E108" s="110" t="s">
+        <v>177</v>
+      </c>
+      <c r="F108" s="110">
+        <v>1</v>
+      </c>
+      <c r="G108" s="110"/>
+      <c r="H108" s="110"/>
+      <c r="I108" s="110"/>
+      <c r="J108" s="110"/>
+      <c r="K108" s="110"/>
+      <c r="L108" s="110"/>
+      <c r="M108" s="110"/>
+      <c r="N108" s="107"/>
+      <c r="O108" s="107"/>
+      <c r="P108" s="107"/>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B109" s="107"/>
+      <c r="C109" s="107"/>
+      <c r="D109" s="107"/>
+      <c r="E109" s="110" t="s">
+        <v>178</v>
+      </c>
+      <c r="F109" s="110">
+        <v>2</v>
+      </c>
+      <c r="G109" s="110"/>
+      <c r="H109" s="110"/>
+      <c r="I109" s="110"/>
+      <c r="J109" s="110"/>
+      <c r="K109" s="110"/>
+      <c r="L109" s="110"/>
+      <c r="M109" s="110"/>
+      <c r="N109" s="107"/>
+      <c r="O109" s="107"/>
+      <c r="P109" s="107"/>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B110" s="107"/>
+      <c r="C110" s="107"/>
+      <c r="D110" s="107"/>
+      <c r="E110" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="F110" s="110">
+        <v>4</v>
+      </c>
+      <c r="G110" s="110"/>
+      <c r="H110" s="110"/>
+      <c r="I110" s="110"/>
+      <c r="J110" s="110"/>
+      <c r="K110" s="110"/>
+      <c r="L110" s="110"/>
+      <c r="M110" s="110"/>
+      <c r="N110" s="107"/>
+      <c r="O110" s="107"/>
+      <c r="P110" s="107"/>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B111" s="107"/>
+      <c r="C111" s="107"/>
+      <c r="D111" s="107"/>
+      <c r="E111" s="110" t="s">
+        <v>180</v>
+      </c>
+      <c r="F111" s="110">
+        <f>3.5*4.5</f>
+        <v>15.75</v>
+      </c>
+      <c r="G111" s="110" t="s">
+        <v>181</v>
+      </c>
+      <c r="H111" s="110"/>
+      <c r="I111" s="110"/>
+      <c r="J111" s="110"/>
+      <c r="K111" s="110"/>
+      <c r="L111" s="110"/>
+      <c r="M111" s="110"/>
+      <c r="N111" s="107"/>
+      <c r="O111" s="107"/>
+      <c r="P111" s="107"/>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B112" s="107"/>
+      <c r="C112" s="107"/>
+      <c r="D112" s="107"/>
+      <c r="E112" s="110"/>
+      <c r="F112" s="110"/>
+      <c r="G112" s="110"/>
+      <c r="H112" s="110"/>
+      <c r="I112" s="110"/>
+      <c r="J112" s="110"/>
+      <c r="K112" s="110"/>
+      <c r="L112" s="110"/>
+      <c r="M112" s="110"/>
+      <c r="N112" s="107"/>
+      <c r="O112" s="107"/>
+      <c r="P112" s="107"/>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B113" s="107"/>
+      <c r="C113" s="107"/>
+      <c r="D113" s="107"/>
+      <c r="E113" s="110"/>
+      <c r="F113" s="110"/>
+      <c r="G113" s="110"/>
+      <c r="H113" s="110"/>
+      <c r="I113" s="110"/>
+      <c r="J113" s="110"/>
+      <c r="K113" s="110"/>
+      <c r="L113" s="110"/>
+      <c r="M113" s="110"/>
+      <c r="N113" s="107"/>
+      <c r="O113" s="107"/>
+      <c r="P113" s="107"/>
+    </row>
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B114" s="107"/>
+      <c r="C114" s="107"/>
+      <c r="D114" s="107"/>
+      <c r="E114" s="110"/>
+      <c r="F114" s="110"/>
+      <c r="G114" s="110"/>
+      <c r="H114" s="110"/>
+      <c r="I114" s="110"/>
+      <c r="J114" s="110"/>
+      <c r="K114" s="110"/>
+      <c r="L114" s="110"/>
+      <c r="M114" s="110"/>
+      <c r="N114" s="107"/>
+      <c r="O114" s="107"/>
+      <c r="P114" s="107"/>
+    </row>
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B115" s="107"/>
+      <c r="C115" s="107"/>
+      <c r="D115" s="107"/>
+      <c r="E115" s="110"/>
+      <c r="F115" s="110"/>
+      <c r="G115" s="110"/>
+      <c r="H115" s="110"/>
+      <c r="I115" s="110"/>
+      <c r="J115" s="110"/>
+      <c r="K115" s="110"/>
+      <c r="L115" s="110"/>
+      <c r="M115" s="110"/>
+      <c r="N115" s="107"/>
+      <c r="O115" s="107"/>
+      <c r="P115" s="107"/>
+    </row>
+    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B116" s="107"/>
+      <c r="C116" s="107"/>
+      <c r="D116" s="107"/>
+      <c r="E116" s="110"/>
+      <c r="F116" s="110"/>
+      <c r="G116" s="110"/>
+      <c r="H116" s="110"/>
+      <c r="I116" s="110"/>
+      <c r="J116" s="110"/>
+      <c r="K116" s="110"/>
+      <c r="L116" s="110"/>
+      <c r="M116" s="110"/>
+      <c r="N116" s="107"/>
+      <c r="O116" s="107"/>
+      <c r="P116" s="107"/>
+    </row>
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B117" s="107"/>
+      <c r="C117" s="107"/>
+      <c r="D117" s="107"/>
+      <c r="E117" s="110"/>
+      <c r="F117" s="110"/>
+      <c r="G117" s="110"/>
+      <c r="H117" s="110"/>
+      <c r="I117" s="110"/>
+      <c r="J117" s="110"/>
+      <c r="K117" s="110"/>
+      <c r="L117" s="110"/>
+      <c r="M117" s="110"/>
+      <c r="N117" s="107"/>
+      <c r="O117" s="107"/>
+      <c r="P117" s="107"/>
+    </row>
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B118" s="107"/>
+      <c r="C118" s="107"/>
+      <c r="D118" s="107"/>
+      <c r="E118" s="110"/>
+      <c r="F118" s="110"/>
+      <c r="G118" s="110"/>
+      <c r="H118" s="110"/>
+      <c r="I118" s="110"/>
+      <c r="J118" s="110"/>
+      <c r="K118" s="110"/>
+      <c r="L118" s="110"/>
+      <c r="M118" s="110"/>
+      <c r="N118" s="107"/>
+      <c r="O118" s="107"/>
+      <c r="P118" s="107"/>
+    </row>
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B119" s="107"/>
+      <c r="C119" s="107"/>
+      <c r="D119" s="107"/>
+      <c r="E119" s="110"/>
+      <c r="F119" s="110"/>
+      <c r="G119" s="110"/>
+      <c r="H119" s="110"/>
+      <c r="I119" s="110"/>
+      <c r="J119" s="110"/>
+      <c r="K119" s="110"/>
+      <c r="L119" s="110"/>
+      <c r="M119" s="110"/>
+      <c r="N119" s="107"/>
+      <c r="O119" s="107"/>
+      <c r="P119" s="107"/>
+    </row>
+    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B120" s="107"/>
+      <c r="C120" s="107"/>
+      <c r="D120" s="107"/>
+      <c r="E120" s="110"/>
+      <c r="F120" s="110"/>
+      <c r="G120" s="110"/>
+      <c r="H120" s="110"/>
+      <c r="I120" s="110"/>
+      <c r="J120" s="110"/>
+      <c r="K120" s="110"/>
+      <c r="L120" s="110"/>
+      <c r="M120" s="110"/>
+      <c r="N120" s="107"/>
+      <c r="O120" s="107"/>
+      <c r="P120" s="107"/>
+    </row>
+    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B121" s="107"/>
+      <c r="C121" s="107"/>
+      <c r="D121" s="107"/>
+      <c r="E121" s="110"/>
+      <c r="F121" s="110"/>
+      <c r="G121" s="110"/>
+      <c r="H121" s="110"/>
+      <c r="I121" s="110"/>
+      <c r="J121" s="110"/>
+      <c r="K121" s="110"/>
+      <c r="L121" s="110"/>
+      <c r="M121" s="110"/>
+      <c r="N121" s="107"/>
+      <c r="O121" s="107"/>
+      <c r="P121" s="107"/>
+    </row>
+    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B122" s="107"/>
+      <c r="C122" s="107"/>
+      <c r="D122" s="107"/>
+      <c r="E122" s="107"/>
+      <c r="F122" s="107"/>
+      <c r="G122" s="107"/>
+      <c r="H122" s="107"/>
+      <c r="I122" s="107"/>
+      <c r="J122" s="107"/>
+      <c r="K122" s="107"/>
+      <c r="L122" s="107"/>
+      <c r="M122" s="107"/>
+      <c r="N122" s="107"/>
+      <c r="O122" s="107"/>
+      <c r="P122" s="107"/>
+    </row>
+    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B123" s="107"/>
+      <c r="C123" s="107"/>
+      <c r="D123" s="107"/>
+      <c r="E123" s="107"/>
+      <c r="F123" s="107"/>
+      <c r="G123" s="107"/>
+      <c r="H123" s="107"/>
+      <c r="I123" s="107"/>
+      <c r="J123" s="107"/>
+      <c r="K123" s="107"/>
+      <c r="L123" s="107"/>
+      <c r="M123" s="107"/>
+      <c r="N123" s="107"/>
+      <c r="O123" s="107"/>
+      <c r="P123" s="107"/>
+    </row>
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B124" s="107"/>
+      <c r="C124" s="107"/>
+      <c r="D124" s="107"/>
+      <c r="E124" s="107"/>
+      <c r="F124" s="107"/>
+      <c r="G124" s="107"/>
+      <c r="H124" s="107"/>
+      <c r="I124" s="107"/>
+      <c r="J124" s="107"/>
+      <c r="K124" s="107"/>
+      <c r="L124" s="107"/>
+      <c r="M124" s="107"/>
+      <c r="N124" s="107"/>
+      <c r="O124" s="107"/>
+      <c r="P124" s="107"/>
+    </row>
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B125" s="107"/>
+      <c r="C125" s="107"/>
+      <c r="D125" s="107"/>
+      <c r="E125" s="107"/>
+      <c r="F125" s="107"/>
+      <c r="G125" s="107"/>
+      <c r="H125" s="107"/>
+      <c r="I125" s="107"/>
+      <c r="J125" s="107"/>
+      <c r="K125" s="107"/>
+      <c r="L125" s="107"/>
+      <c r="M125" s="107"/>
+      <c r="N125" s="107"/>
+      <c r="O125" s="107"/>
+      <c r="P125" s="107"/>
+    </row>
+    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B126" s="107"/>
+      <c r="C126" s="107"/>
+      <c r="D126" s="107"/>
+      <c r="E126" s="107"/>
+      <c r="F126" s="107"/>
+      <c r="G126" s="107"/>
+      <c r="H126" s="107"/>
+      <c r="I126" s="107"/>
+      <c r="J126" s="107"/>
+      <c r="K126" s="107"/>
+      <c r="L126" s="107"/>
+      <c r="M126" s="107"/>
+      <c r="N126" s="107"/>
+      <c r="O126" s="107"/>
+      <c r="P126" s="107"/>
+    </row>
+    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B127" s="107"/>
+      <c r="C127" s="107"/>
+      <c r="D127" s="107"/>
+      <c r="E127" s="107"/>
+      <c r="F127" s="107"/>
+      <c r="G127" s="107"/>
+      <c r="H127" s="107"/>
+      <c r="I127" s="107"/>
+      <c r="J127" s="107"/>
+      <c r="K127" s="107"/>
+      <c r="L127" s="107"/>
+      <c r="M127" s="107"/>
+      <c r="N127" s="107"/>
+      <c r="O127" s="107"/>
+      <c r="P127" s="107"/>
+    </row>
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B128" s="107"/>
+      <c r="C128" s="107"/>
+      <c r="D128" s="107"/>
+      <c r="E128" s="107"/>
+      <c r="F128" s="107"/>
+      <c r="G128" s="107"/>
+      <c r="H128" s="107"/>
+      <c r="I128" s="107"/>
+      <c r="J128" s="107"/>
+      <c r="K128" s="107"/>
+      <c r="L128" s="107"/>
+      <c r="M128" s="107"/>
+      <c r="N128" s="107"/>
+      <c r="O128" s="107"/>
+      <c r="P128" s="107"/>
+    </row>
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B129" s="107"/>
+      <c r="C129" s="107"/>
+      <c r="D129" s="107"/>
+      <c r="E129" s="107"/>
+      <c r="F129" s="107"/>
+      <c r="G129" s="107"/>
+      <c r="H129" s="107"/>
+      <c r="I129" s="107"/>
+      <c r="J129" s="107"/>
+      <c r="K129" s="107"/>
+      <c r="L129" s="107"/>
+      <c r="M129" s="107"/>
+      <c r="N129" s="107"/>
+      <c r="O129" s="107"/>
+      <c r="P129" s="107"/>
+    </row>
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B130" s="107"/>
+      <c r="C130" s="107"/>
+      <c r="D130" s="107"/>
+      <c r="E130" s="107"/>
+      <c r="F130" s="107"/>
+      <c r="G130" s="107"/>
+      <c r="H130" s="107"/>
+      <c r="I130" s="107"/>
+      <c r="J130" s="107"/>
+      <c r="K130" s="107"/>
+      <c r="L130" s="107"/>
+      <c r="M130" s="107"/>
+      <c r="N130" s="107"/>
+      <c r="O130" s="107"/>
+      <c r="P130" s="107"/>
+    </row>
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B131" s="107"/>
+      <c r="C131" s="107"/>
+      <c r="D131" s="107"/>
+      <c r="E131" s="107"/>
+      <c r="F131" s="107"/>
+      <c r="G131" s="107"/>
+      <c r="H131" s="107"/>
+      <c r="I131" s="107"/>
+      <c r="J131" s="107"/>
+      <c r="K131" s="107"/>
+      <c r="L131" s="107"/>
+      <c r="M131" s="107"/>
+      <c r="N131" s="107"/>
+      <c r="O131" s="107"/>
+      <c r="P131" s="107"/>
+    </row>
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B132" s="107"/>
+      <c r="C132" s="107"/>
+      <c r="D132" s="107"/>
+      <c r="E132" s="107"/>
+      <c r="F132" s="107"/>
+      <c r="G132" s="107"/>
+      <c r="H132" s="107"/>
+      <c r="I132" s="107"/>
+      <c r="J132" s="107"/>
+      <c r="K132" s="107"/>
+      <c r="L132" s="107"/>
+      <c r="M132" s="107"/>
+      <c r="N132" s="107"/>
+      <c r="O132" s="107"/>
+      <c r="P132" s="107"/>
+    </row>
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B133" s="107"/>
+      <c r="C133" s="107"/>
+      <c r="D133" s="107"/>
+      <c r="E133" s="107"/>
+      <c r="F133" s="107"/>
+      <c r="G133" s="107"/>
+      <c r="H133" s="107"/>
+      <c r="I133" s="107"/>
+      <c r="J133" s="107"/>
+      <c r="K133" s="107"/>
+      <c r="L133" s="107"/>
+      <c r="M133" s="107"/>
+      <c r="N133" s="107"/>
+      <c r="O133" s="107"/>
+      <c r="P133" s="107"/>
+    </row>
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B134" s="107"/>
+      <c r="C134" s="107"/>
+      <c r="D134" s="107"/>
+      <c r="E134" s="107"/>
+      <c r="F134" s="107"/>
+      <c r="G134" s="107"/>
+      <c r="H134" s="107"/>
+      <c r="I134" s="107"/>
+      <c r="J134" s="107"/>
+      <c r="K134" s="107"/>
+      <c r="L134" s="107"/>
+      <c r="M134" s="107"/>
+      <c r="N134" s="107"/>
+      <c r="O134" s="107"/>
+      <c r="P134" s="107"/>
+    </row>
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B135" s="107"/>
+      <c r="C135" s="107"/>
+      <c r="D135" s="107"/>
+      <c r="E135" s="107"/>
+      <c r="F135" s="107"/>
+      <c r="G135" s="107"/>
+      <c r="H135" s="107"/>
+      <c r="I135" s="107"/>
+      <c r="J135" s="107"/>
+      <c r="K135" s="107"/>
+      <c r="L135" s="107"/>
+      <c r="M135" s="107"/>
+      <c r="N135" s="107"/>
+      <c r="O135" s="107"/>
+      <c r="P135" s="107"/>
+    </row>
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B136" s="107"/>
+      <c r="C136" s="107"/>
+      <c r="D136" s="107"/>
+      <c r="E136" s="107"/>
+      <c r="F136" s="107"/>
+      <c r="G136" s="107"/>
+      <c r="H136" s="107"/>
+      <c r="I136" s="107"/>
+      <c r="J136" s="107"/>
+      <c r="K136" s="107"/>
+      <c r="L136" s="107"/>
+      <c r="M136" s="107"/>
+      <c r="N136" s="107"/>
+      <c r="O136" s="107"/>
+      <c r="P136" s="107"/>
+    </row>
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B137" s="107"/>
+      <c r="C137" s="107"/>
+      <c r="D137" s="107"/>
+      <c r="E137" s="107"/>
+      <c r="F137" s="107"/>
+      <c r="G137" s="107"/>
+      <c r="H137" s="107"/>
+      <c r="I137" s="107"/>
+      <c r="J137" s="107"/>
+      <c r="K137" s="107"/>
+      <c r="L137" s="107"/>
+      <c r="M137" s="107"/>
+      <c r="N137" s="107"/>
+      <c r="O137" s="107"/>
+      <c r="P137" s="107"/>
+    </row>
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B138" s="107"/>
+      <c r="C138" s="107"/>
+      <c r="D138" s="107"/>
+      <c r="E138" s="107"/>
+      <c r="F138" s="107"/>
+      <c r="G138" s="107"/>
+      <c r="H138" s="107"/>
+      <c r="I138" s="107"/>
+      <c r="J138" s="107"/>
+      <c r="K138" s="107"/>
+      <c r="L138" s="107"/>
+      <c r="M138" s="107"/>
+      <c r="N138" s="107"/>
+      <c r="O138" s="107"/>
+      <c r="P138" s="107"/>
+    </row>
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B139" s="107"/>
+      <c r="C139" s="107"/>
+      <c r="D139" s="107"/>
+      <c r="E139" s="107"/>
+      <c r="F139" s="107"/>
+      <c r="G139" s="107"/>
+      <c r="H139" s="107"/>
+      <c r="I139" s="107"/>
+      <c r="J139" s="107"/>
+      <c r="K139" s="107"/>
+      <c r="L139" s="107"/>
+      <c r="M139" s="107"/>
+      <c r="N139" s="107"/>
+      <c r="O139" s="107"/>
+      <c r="P139" s="107"/>
+    </row>
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B140" s="107"/>
+      <c r="C140" s="107"/>
+      <c r="D140" s="107"/>
+      <c r="E140" s="107"/>
+      <c r="F140" s="107"/>
+      <c r="G140" s="107"/>
+      <c r="H140" s="107"/>
+      <c r="I140" s="107"/>
+      <c r="J140" s="107"/>
+      <c r="K140" s="107"/>
+      <c r="L140" s="107"/>
+      <c r="M140" s="107"/>
+      <c r="N140" s="107"/>
+      <c r="O140" s="107"/>
+      <c r="P140" s="107"/>
+    </row>
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B141" s="107"/>
+      <c r="C141" s="107"/>
+      <c r="D141" s="107"/>
+      <c r="E141" s="107"/>
+      <c r="F141" s="107"/>
+      <c r="G141" s="107"/>
+      <c r="H141" s="107"/>
+      <c r="I141" s="107"/>
+      <c r="J141" s="107"/>
+      <c r="K141" s="107"/>
+      <c r="L141" s="107"/>
+      <c r="M141" s="107"/>
+      <c r="N141" s="107"/>
+      <c r="O141" s="107"/>
+      <c r="P141" s="107"/>
+    </row>
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B142" s="107"/>
+      <c r="C142" s="107"/>
+      <c r="D142" s="107"/>
+      <c r="E142" s="107"/>
+      <c r="F142" s="107"/>
+      <c r="G142" s="107"/>
+      <c r="H142" s="107"/>
+      <c r="I142" s="107"/>
+      <c r="J142" s="107"/>
+      <c r="K142" s="107"/>
+      <c r="L142" s="107"/>
+      <c r="M142" s="107"/>
+      <c r="N142" s="107"/>
+      <c r="O142" s="107"/>
+      <c r="P142" s="107"/>
+    </row>
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B143" s="107"/>
+      <c r="C143" s="107"/>
+      <c r="D143" s="107"/>
+      <c r="E143" s="107"/>
+      <c r="F143" s="107"/>
+      <c r="G143" s="107"/>
+      <c r="H143" s="107"/>
+      <c r="I143" s="107"/>
+      <c r="J143" s="107"/>
+      <c r="K143" s="107"/>
+      <c r="L143" s="107"/>
+      <c r="M143" s="107"/>
+      <c r="N143" s="107"/>
+      <c r="O143" s="107"/>
+      <c r="P143" s="107"/>
+    </row>
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B144" s="107"/>
+      <c r="C144" s="107"/>
+      <c r="D144" s="107"/>
+      <c r="E144" s="107"/>
+      <c r="F144" s="107"/>
+      <c r="G144" s="107"/>
+      <c r="H144" s="107"/>
+      <c r="I144" s="107"/>
+      <c r="J144" s="107"/>
+      <c r="K144" s="107"/>
+      <c r="L144" s="107"/>
+      <c r="M144" s="107"/>
+      <c r="N144" s="107"/>
+      <c r="O144" s="107"/>
+      <c r="P144" s="107"/>
+    </row>
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B145" s="107"/>
+      <c r="C145" s="107"/>
+      <c r="D145" s="107"/>
+      <c r="E145" s="107"/>
+      <c r="F145" s="107"/>
+      <c r="G145" s="107"/>
+      <c r="H145" s="107"/>
+      <c r="I145" s="107"/>
+      <c r="J145" s="107"/>
+      <c r="K145" s="107"/>
+      <c r="L145" s="107"/>
+      <c r="M145" s="107"/>
+      <c r="N145" s="107"/>
+      <c r="O145" s="107"/>
+      <c r="P145" s="107"/>
+    </row>
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B146" s="107"/>
+      <c r="C146" s="107"/>
+      <c r="D146" s="107"/>
+      <c r="E146" s="107"/>
+      <c r="F146" s="107"/>
+      <c r="G146" s="107"/>
+      <c r="H146" s="107"/>
+      <c r="I146" s="107"/>
+      <c r="J146" s="107"/>
+      <c r="K146" s="107"/>
+      <c r="L146" s="107"/>
+      <c r="M146" s="107"/>
+      <c r="N146" s="107"/>
+      <c r="O146" s="107"/>
+      <c r="P146" s="107"/>
+    </row>
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B147" s="107"/>
+      <c r="C147" s="107"/>
+      <c r="D147" s="107"/>
+      <c r="E147" s="107"/>
+      <c r="F147" s="107"/>
+      <c r="G147" s="107"/>
+      <c r="H147" s="107"/>
+      <c r="I147" s="107"/>
+      <c r="J147" s="107"/>
+      <c r="K147" s="107"/>
+      <c r="L147" s="107"/>
+      <c r="M147" s="107"/>
+      <c r="N147" s="107"/>
+      <c r="O147" s="107"/>
+      <c r="P147" s="107"/>
+    </row>
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B148" s="107"/>
+      <c r="C148" s="107"/>
+      <c r="D148" s="107"/>
+      <c r="E148" s="107"/>
+      <c r="F148" s="107"/>
+      <c r="G148" s="107"/>
+      <c r="H148" s="107"/>
+      <c r="I148" s="107"/>
+      <c r="J148" s="107"/>
+      <c r="K148" s="107"/>
+      <c r="L148" s="107"/>
+      <c r="M148" s="107"/>
+      <c r="N148" s="107"/>
+      <c r="O148" s="107"/>
+      <c r="P148" s="107"/>
+    </row>
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B149" s="107"/>
+      <c r="C149" s="107"/>
+      <c r="D149" s="107"/>
+      <c r="E149" s="107"/>
+      <c r="F149" s="107"/>
+      <c r="G149" s="107"/>
+      <c r="H149" s="107"/>
+      <c r="I149" s="107"/>
+      <c r="J149" s="107"/>
+      <c r="K149" s="107"/>
+      <c r="L149" s="107"/>
+      <c r="M149" s="107"/>
+      <c r="N149" s="107"/>
+      <c r="O149" s="107"/>
+      <c r="P149" s="107"/>
+    </row>
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B150" s="107"/>
+      <c r="C150" s="107"/>
+      <c r="D150" s="107"/>
+      <c r="E150" s="107"/>
+      <c r="F150" s="107"/>
+      <c r="G150" s="107"/>
+      <c r="H150" s="107"/>
+      <c r="I150" s="107"/>
+      <c r="J150" s="107"/>
+      <c r="K150" s="107"/>
+      <c r="L150" s="107"/>
+      <c r="M150" s="107"/>
+      <c r="N150" s="107"/>
+      <c r="O150" s="107"/>
+      <c r="P150" s="107"/>
+    </row>
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B151" s="107"/>
+      <c r="C151" s="107"/>
+      <c r="D151" s="107"/>
+      <c r="E151" s="107"/>
+      <c r="F151" s="107"/>
+      <c r="G151" s="107"/>
+      <c r="H151" s="107"/>
+      <c r="I151" s="107"/>
+      <c r="J151" s="107"/>
+      <c r="K151" s="107"/>
+      <c r="L151" s="107"/>
+      <c r="M151" s="107"/>
+      <c r="N151" s="107"/>
+      <c r="O151" s="107"/>
+      <c r="P151" s="107"/>
+    </row>
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B152" s="107"/>
+      <c r="C152" s="107"/>
+      <c r="D152" s="107"/>
+      <c r="E152" s="107"/>
+      <c r="F152" s="107"/>
+      <c r="G152" s="107"/>
+      <c r="H152" s="107"/>
+      <c r="I152" s="107"/>
+      <c r="J152" s="107"/>
+      <c r="K152" s="107"/>
+      <c r="L152" s="107"/>
+      <c r="M152" s="107"/>
+      <c r="N152" s="107"/>
+      <c r="O152" s="107"/>
+      <c r="P152" s="107"/>
+    </row>
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B153" s="107"/>
+      <c r="C153" s="107"/>
+      <c r="D153" s="107"/>
+      <c r="E153" s="107"/>
+      <c r="F153" s="107"/>
+      <c r="G153" s="107"/>
+      <c r="H153" s="107"/>
+      <c r="I153" s="107"/>
+      <c r="J153" s="107"/>
+      <c r="K153" s="107"/>
+      <c r="L153" s="107"/>
+      <c r="M153" s="107"/>
+      <c r="N153" s="107"/>
+      <c r="O153" s="107"/>
+      <c r="P153" s="107"/>
+    </row>
   </sheetData>
-  <mergeCells count="74">
+  <mergeCells count="77">
+    <mergeCell ref="E79:G82"/>
+    <mergeCell ref="H79:J82"/>
+    <mergeCell ref="K79:M82"/>
+    <mergeCell ref="D71:R71"/>
+    <mergeCell ref="B71:C75"/>
+    <mergeCell ref="A57:C58"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="A16:V16"/>
+    <mergeCell ref="A37:R37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="M38:Q38"/>
+    <mergeCell ref="F57:G58"/>
+    <mergeCell ref="H57:I58"/>
+    <mergeCell ref="D57:E58"/>
+    <mergeCell ref="J57:O58"/>
+    <mergeCell ref="T55:V58"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="T64:V64"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="A55:S56"/>
+    <mergeCell ref="P57:S58"/>
+    <mergeCell ref="P59:S59"/>
+    <mergeCell ref="P60:S60"/>
+    <mergeCell ref="P61:S61"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="J60:O60"/>
+    <mergeCell ref="J61:O61"/>
+    <mergeCell ref="J62:O62"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H64:I64"/>
     <mergeCell ref="T65:V65"/>
     <mergeCell ref="T67:V67"/>
     <mergeCell ref="T66:V66"/>
@@ -5436,64 +7164,6 @@
     <mergeCell ref="T61:V61"/>
     <mergeCell ref="T62:V62"/>
     <mergeCell ref="J64:O64"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="T64:V64"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="A55:S56"/>
-    <mergeCell ref="P57:S58"/>
-    <mergeCell ref="P59:S59"/>
-    <mergeCell ref="P60:S60"/>
-    <mergeCell ref="P61:S61"/>
-    <mergeCell ref="J59:O59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="J60:O60"/>
-    <mergeCell ref="J61:O61"/>
-    <mergeCell ref="J62:O62"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="D71:R71"/>
-    <mergeCell ref="B71:C75"/>
-    <mergeCell ref="A57:C58"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="A16:V16"/>
-    <mergeCell ref="A37:R37"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="M38:Q38"/>
-    <mergeCell ref="F57:G58"/>
-    <mergeCell ref="H57:I58"/>
-    <mergeCell ref="D57:E58"/>
-    <mergeCell ref="J57:O58"/>
-    <mergeCell ref="T55:V58"/>
-    <mergeCell ref="H59:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
-realizarea coroanei rotii cilindrice
-trebuie modificata pana din forma B in forma C
</commit_message>
<xml_diff>
--- a/PROIECT OM2 CALCULE.xlsx
+++ b/PROIECT OM2 CALCULE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reductor-Conico-Cilindric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D33B67-3E15-4972-B2EE-C0F1E7A81674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666CD3EC-A6D2-4651-8337-742581061268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2143,6 +2143,81 @@
     <xf numFmtId="164" fontId="0" fillId="24" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="17" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="17" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="8" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="23" fillId="23" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2168,81 +2243,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="6" borderId="0" xfId="4" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="8" borderId="8" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="8" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="17" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="10" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="22" fillId="17" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="15" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3197,8 +3197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q89" sqref="Q89"/>
+    <sheetView tabSelected="1" topLeftCell="C76" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G119" sqref="G119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3236,23 +3236,23 @@
       <c r="B1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="100" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="103" t="s">
+      <c r="E1" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -3261,15 +3261,15 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="104"/>
+      <c r="C2" s="101"/>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
@@ -3521,30 +3521,30 @@
       <c r="V15" s="15"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="96" t="s">
+      <c r="A16" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="96"/>
-      <c r="J16" s="96"/>
-      <c r="K16" s="96"/>
-      <c r="L16" s="96"/>
-      <c r="M16" s="96"/>
-      <c r="N16" s="96"/>
-      <c r="O16" s="96"/>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="96"/>
-      <c r="S16" s="96"/>
-      <c r="T16" s="96"/>
-      <c r="U16" s="96"/>
-      <c r="V16" s="96"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="105"/>
+      <c r="Q16" s="105"/>
+      <c r="R16" s="105"/>
+      <c r="S16" s="105"/>
+      <c r="T16" s="105"/>
+      <c r="U16" s="105"/>
+      <c r="V16" s="105"/>
     </row>
     <row r="17" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
@@ -3552,18 +3552,18 @@
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="95" t="s">
+      <c r="F17" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95" t="s">
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="95"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
       <c r="P17" s="15"/>
@@ -3605,10 +3605,10 @@
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="15"/>
-      <c r="O18" s="98" t="s">
+      <c r="O18" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="P18" s="98"/>
+      <c r="P18" s="107"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
@@ -4047,12 +4047,12 @@
       <c r="V28" s="15"/>
     </row>
     <row r="29" spans="1:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="105" t="s">
+      <c r="A29" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
+      <c r="D29" s="103"/>
       <c r="E29" s="15"/>
       <c r="F29" s="16"/>
       <c r="G29" s="29" t="s">
@@ -4282,26 +4282,26 @@
       <c r="V34" s="15"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="97" t="s">
+      <c r="A37" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="97"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="97"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="97"/>
-      <c r="K37" s="97"/>
-      <c r="L37" s="97"/>
-      <c r="M37" s="97"/>
-      <c r="N37" s="97"/>
-      <c r="O37" s="97"/>
-      <c r="P37" s="97"/>
-      <c r="Q37" s="97"/>
-      <c r="R37" s="97"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="106"/>
+      <c r="D37" s="106"/>
+      <c r="E37" s="106"/>
+      <c r="F37" s="106"/>
+      <c r="G37" s="106"/>
+      <c r="H37" s="106"/>
+      <c r="I37" s="106"/>
+      <c r="J37" s="106"/>
+      <c r="K37" s="106"/>
+      <c r="L37" s="106"/>
+      <c r="M37" s="106"/>
+      <c r="N37" s="106"/>
+      <c r="O37" s="106"/>
+      <c r="P37" s="106"/>
+      <c r="Q37" s="106"/>
+      <c r="R37" s="106"/>
       <c r="S37" s="39"/>
       <c r="T37" s="39"/>
       <c r="U37" s="39"/>
@@ -4318,25 +4318,25 @@
       <c r="D38" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E38" s="94" t="s">
+      <c r="E38" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="F38" s="94"/>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="94" t="s">
+      <c r="F38" s="104"/>
+      <c r="G38" s="104"/>
+      <c r="H38" s="104"/>
+      <c r="I38" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="J38" s="94"/>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="99" t="s">
+      <c r="J38" s="104"/>
+      <c r="K38" s="104"/>
+      <c r="L38" s="104"/>
+      <c r="M38" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="N38" s="99"/>
-      <c r="O38" s="99"/>
-      <c r="P38" s="99"/>
-      <c r="Q38" s="99"/>
+      <c r="N38" s="108"/>
+      <c r="O38" s="108"/>
+      <c r="P38" s="108"/>
+      <c r="Q38" s="108"/>
       <c r="R38" s="39"/>
       <c r="S38" s="39"/>
       <c r="T38" s="39"/>
@@ -5017,120 +5017,120 @@
       <c r="V54" s="39"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A55" s="112" t="s">
+      <c r="A55" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="112"/>
-      <c r="C55" s="112"/>
-      <c r="D55" s="112"/>
-      <c r="E55" s="112"/>
-      <c r="F55" s="112"/>
-      <c r="G55" s="112"/>
-      <c r="H55" s="112"/>
-      <c r="I55" s="112"/>
-      <c r="J55" s="112"/>
-      <c r="K55" s="112"/>
-      <c r="L55" s="112"/>
-      <c r="M55" s="112"/>
-      <c r="N55" s="112"/>
-      <c r="O55" s="112"/>
-      <c r="P55" s="112"/>
-      <c r="Q55" s="112"/>
-      <c r="R55" s="112"/>
-      <c r="S55" s="112"/>
-      <c r="T55" s="101" t="s">
+      <c r="B55" s="94"/>
+      <c r="C55" s="94"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="94"/>
+      <c r="G55" s="94"/>
+      <c r="H55" s="94"/>
+      <c r="I55" s="94"/>
+      <c r="J55" s="94"/>
+      <c r="K55" s="94"/>
+      <c r="L55" s="94"/>
+      <c r="M55" s="94"/>
+      <c r="N55" s="94"/>
+      <c r="O55" s="94"/>
+      <c r="P55" s="94"/>
+      <c r="Q55" s="94"/>
+      <c r="R55" s="94"/>
+      <c r="S55" s="94"/>
+      <c r="T55" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="U55" s="101"/>
-      <c r="V55" s="101"/>
-      <c r="W55" s="117"/>
+      <c r="U55" s="109"/>
+      <c r="V55" s="109"/>
+      <c r="W55" s="88"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A56" s="112"/>
-      <c r="B56" s="112"/>
-      <c r="C56" s="112"/>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112"/>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112"/>
-      <c r="H56" s="112"/>
-      <c r="I56" s="112"/>
-      <c r="J56" s="112"/>
-      <c r="K56" s="112"/>
-      <c r="L56" s="112"/>
-      <c r="M56" s="112"/>
-      <c r="N56" s="112"/>
-      <c r="O56" s="112"/>
-      <c r="P56" s="112"/>
-      <c r="Q56" s="112"/>
-      <c r="R56" s="112"/>
-      <c r="S56" s="112"/>
-      <c r="T56" s="101"/>
-      <c r="U56" s="101"/>
-      <c r="V56" s="101"/>
-      <c r="W56" s="117"/>
+      <c r="A56" s="94"/>
+      <c r="B56" s="94"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="94"/>
+      <c r="E56" s="94"/>
+      <c r="F56" s="94"/>
+      <c r="G56" s="94"/>
+      <c r="H56" s="94"/>
+      <c r="I56" s="94"/>
+      <c r="J56" s="94"/>
+      <c r="K56" s="94"/>
+      <c r="L56" s="94"/>
+      <c r="M56" s="94"/>
+      <c r="N56" s="94"/>
+      <c r="O56" s="94"/>
+      <c r="P56" s="94"/>
+      <c r="Q56" s="94"/>
+      <c r="R56" s="94"/>
+      <c r="S56" s="94"/>
+      <c r="T56" s="109"/>
+      <c r="U56" s="109"/>
+      <c r="V56" s="109"/>
+      <c r="W56" s="88"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A57" s="94" t="s">
+      <c r="A57" s="104" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="94"/>
-      <c r="C57" s="94"/>
-      <c r="D57" s="100" t="s">
+      <c r="B57" s="104"/>
+      <c r="C57" s="104"/>
+      <c r="D57" s="95" t="s">
         <v>125</v>
       </c>
-      <c r="E57" s="100"/>
-      <c r="F57" s="100" t="s">
+      <c r="E57" s="95"/>
+      <c r="F57" s="95" t="s">
         <v>127</v>
       </c>
-      <c r="G57" s="100"/>
-      <c r="H57" s="100" t="s">
+      <c r="G57" s="95"/>
+      <c r="H57" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="I57" s="100"/>
-      <c r="J57" s="100" t="s">
+      <c r="I57" s="95"/>
+      <c r="J57" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="K57" s="100"/>
-      <c r="L57" s="100"/>
-      <c r="M57" s="100"/>
-      <c r="N57" s="100"/>
-      <c r="O57" s="100"/>
-      <c r="P57" s="100" t="s">
+      <c r="K57" s="95"/>
+      <c r="L57" s="95"/>
+      <c r="M57" s="95"/>
+      <c r="N57" s="95"/>
+      <c r="O57" s="95"/>
+      <c r="P57" s="95" t="s">
         <v>126</v>
       </c>
-      <c r="Q57" s="100"/>
-      <c r="R57" s="100"/>
-      <c r="S57" s="113"/>
-      <c r="T57" s="101"/>
-      <c r="U57" s="101"/>
-      <c r="V57" s="101"/>
-      <c r="W57" s="117"/>
+      <c r="Q57" s="95"/>
+      <c r="R57" s="95"/>
+      <c r="S57" s="96"/>
+      <c r="T57" s="109"/>
+      <c r="U57" s="109"/>
+      <c r="V57" s="109"/>
+      <c r="W57" s="88"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A58" s="94"/>
-      <c r="B58" s="94"/>
-      <c r="C58" s="94"/>
-      <c r="D58" s="100"/>
-      <c r="E58" s="100"/>
-      <c r="F58" s="100"/>
-      <c r="G58" s="100"/>
-      <c r="H58" s="100"/>
-      <c r="I58" s="100"/>
-      <c r="J58" s="100"/>
-      <c r="K58" s="100"/>
-      <c r="L58" s="100"/>
-      <c r="M58" s="100"/>
-      <c r="N58" s="100"/>
-      <c r="O58" s="100"/>
-      <c r="P58" s="100"/>
-      <c r="Q58" s="100"/>
-      <c r="R58" s="100"/>
-      <c r="S58" s="113"/>
-      <c r="T58" s="101"/>
-      <c r="U58" s="101"/>
-      <c r="V58" s="101"/>
-      <c r="W58" s="117"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="104"/>
+      <c r="C58" s="104"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="95"/>
+      <c r="H58" s="95"/>
+      <c r="I58" s="95"/>
+      <c r="J58" s="95"/>
+      <c r="K58" s="95"/>
+      <c r="L58" s="95"/>
+      <c r="M58" s="95"/>
+      <c r="N58" s="95"/>
+      <c r="O58" s="95"/>
+      <c r="P58" s="95"/>
+      <c r="Q58" s="95"/>
+      <c r="R58" s="95"/>
+      <c r="S58" s="96"/>
+      <c r="T58" s="109"/>
+      <c r="U58" s="109"/>
+      <c r="V58" s="109"/>
+      <c r="W58" s="88"/>
     </row>
     <row r="59" spans="1:23" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="69" t="s">
@@ -5142,39 +5142,39 @@
       <c r="C59" s="71">
         <v>20.646896487046401</v>
       </c>
-      <c r="D59" s="102">
+      <c r="D59" s="90">
         <v>16</v>
       </c>
-      <c r="E59" s="102"/>
-      <c r="F59" s="102">
+      <c r="E59" s="90"/>
+      <c r="F59" s="90">
         <v>62</v>
       </c>
-      <c r="G59" s="102"/>
-      <c r="H59" s="102">
+      <c r="G59" s="90"/>
+      <c r="H59" s="90">
         <f>F59/D59</f>
         <v>3.875</v>
       </c>
-      <c r="I59" s="102"/>
-      <c r="J59" s="102">
+      <c r="I59" s="90"/>
+      <c r="J59" s="90">
         <f>((G7-H59)/C39)*100</f>
         <v>0</v>
       </c>
-      <c r="K59" s="102"/>
-      <c r="L59" s="102"/>
-      <c r="M59" s="102"/>
-      <c r="N59" s="102"/>
-      <c r="O59" s="102"/>
-      <c r="P59" s="102">
+      <c r="K59" s="90"/>
+      <c r="L59" s="90"/>
+      <c r="M59" s="90"/>
+      <c r="N59" s="90"/>
+      <c r="O59" s="90"/>
+      <c r="P59" s="90">
         <v>222.0667</v>
       </c>
-      <c r="Q59" s="102"/>
-      <c r="R59" s="102"/>
-      <c r="S59" s="114"/>
-      <c r="T59" s="102" t="s">
+      <c r="Q59" s="90"/>
+      <c r="R59" s="90"/>
+      <c r="S59" s="97"/>
+      <c r="T59" s="90" t="s">
         <v>135</v>
       </c>
-      <c r="U59" s="102"/>
-      <c r="V59" s="102"/>
+      <c r="U59" s="90"/>
+      <c r="V59" s="90"/>
     </row>
     <row r="60" spans="1:23" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="69" t="s">
@@ -5186,40 +5186,40 @@
       <c r="C60" s="72">
         <v>22.546048321514299</v>
       </c>
-      <c r="D60" s="106">
+      <c r="D60" s="98">
         <v>16</v>
       </c>
-      <c r="E60" s="106"/>
-      <c r="F60" s="106">
+      <c r="E60" s="98"/>
+      <c r="F60" s="98">
         <v>63</v>
       </c>
-      <c r="G60" s="106"/>
-      <c r="H60" s="106">
+      <c r="G60" s="98"/>
+      <c r="H60" s="98">
         <f>F60/D60</f>
         <v>3.9375</v>
       </c>
-      <c r="I60" s="106"/>
-      <c r="J60" s="106">
+      <c r="I60" s="98"/>
+      <c r="J60" s="98">
         <f>((G7-H60)/C$39)*100</f>
         <v>-1.6129032258064515</v>
       </c>
-      <c r="K60" s="106"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="106"/>
-      <c r="N60" s="106"/>
-      <c r="O60" s="106"/>
-      <c r="P60" s="106">
+      <c r="K60" s="98"/>
+      <c r="L60" s="98"/>
+      <c r="M60" s="98"/>
+      <c r="N60" s="98"/>
+      <c r="O60" s="98"/>
+      <c r="P60" s="98">
         <v>224.91374999999999</v>
       </c>
-      <c r="Q60" s="106"/>
-      <c r="R60" s="106"/>
-      <c r="S60" s="115"/>
-      <c r="T60" s="118" t="b">
+      <c r="Q60" s="98"/>
+      <c r="R60" s="98"/>
+      <c r="S60" s="99"/>
+      <c r="T60" s="91" t="b">
         <f>-2.75&lt;0.08625&lt;5.5</f>
         <v>0</v>
       </c>
-      <c r="U60" s="118"/>
-      <c r="V60" s="118"/>
+      <c r="U60" s="91"/>
+      <c r="V60" s="91"/>
       <c r="W60" s="39">
         <f>225-P60</f>
         <v>8.6250000000006821E-2</v>
@@ -5235,40 +5235,40 @@
       <c r="C61" s="72">
         <v>0.55711257339562903</v>
       </c>
-      <c r="D61" s="107">
+      <c r="D61" s="92">
         <v>17</v>
       </c>
-      <c r="E61" s="107"/>
-      <c r="F61" s="107">
+      <c r="E61" s="92"/>
+      <c r="F61" s="92">
         <v>62</v>
       </c>
-      <c r="G61" s="107"/>
-      <c r="H61" s="107">
+      <c r="G61" s="92"/>
+      <c r="H61" s="92">
         <f>F61/D61</f>
         <v>3.6470588235294117</v>
       </c>
-      <c r="I61" s="107"/>
-      <c r="J61" s="107">
+      <c r="I61" s="92"/>
+      <c r="J61" s="92">
         <f>((G7-H61)/G7)*100</f>
         <v>5.8823529411764728</v>
       </c>
-      <c r="K61" s="107"/>
-      <c r="L61" s="107"/>
-      <c r="M61" s="107"/>
-      <c r="N61" s="107"/>
-      <c r="O61" s="107"/>
-      <c r="P61" s="107">
+      <c r="K61" s="92"/>
+      <c r="L61" s="92"/>
+      <c r="M61" s="92"/>
+      <c r="N61" s="92"/>
+      <c r="O61" s="92"/>
+      <c r="P61" s="92">
         <v>224.91374999999999</v>
       </c>
-      <c r="Q61" s="107"/>
-      <c r="R61" s="107"/>
-      <c r="S61" s="111"/>
-      <c r="T61" s="118" t="b">
+      <c r="Q61" s="92"/>
+      <c r="R61" s="92"/>
+      <c r="S61" s="93"/>
+      <c r="T61" s="91" t="b">
         <f>-0.5*5.5&lt;225-P61&lt;=5.5</f>
         <v>0</v>
       </c>
-      <c r="U61" s="118"/>
-      <c r="V61" s="118"/>
+      <c r="U61" s="91"/>
+      <c r="V61" s="91"/>
     </row>
     <row r="62" spans="1:23" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="69" t="s">
@@ -5280,40 +5280,40 @@
       <c r="C62" s="72">
         <v>0.410419384902517</v>
       </c>
-      <c r="D62" s="107">
+      <c r="D62" s="92">
         <v>17</v>
       </c>
-      <c r="E62" s="107"/>
-      <c r="F62" s="107">
+      <c r="E62" s="92"/>
+      <c r="F62" s="92">
         <v>63</v>
       </c>
-      <c r="G62" s="107"/>
-      <c r="H62" s="107">
+      <c r="G62" s="92"/>
+      <c r="H62" s="92">
         <f>F62/D62</f>
         <v>3.7058823529411766</v>
       </c>
-      <c r="I62" s="107"/>
-      <c r="J62" s="107">
+      <c r="I62" s="92"/>
+      <c r="J62" s="92">
         <f>((G7-H62)/C39)*100</f>
         <v>4.3643263757115713</v>
       </c>
-      <c r="K62" s="107"/>
-      <c r="L62" s="107"/>
-      <c r="M62" s="107"/>
-      <c r="N62" s="107"/>
-      <c r="O62" s="107"/>
-      <c r="P62" s="107">
+      <c r="K62" s="92"/>
+      <c r="L62" s="92"/>
+      <c r="M62" s="92"/>
+      <c r="N62" s="92"/>
+      <c r="O62" s="92"/>
+      <c r="P62" s="92">
         <v>227.76075968999999</v>
       </c>
-      <c r="Q62" s="107"/>
-      <c r="R62" s="107"/>
-      <c r="S62" s="111"/>
-      <c r="T62" s="118" t="b">
+      <c r="Q62" s="92"/>
+      <c r="R62" s="92"/>
+      <c r="S62" s="93"/>
+      <c r="T62" s="91" t="b">
         <f>-0.5*5.5&lt;225-P62&lt;=5.5</f>
         <v>0</v>
       </c>
-      <c r="U62" s="118"/>
-      <c r="V62" s="118"/>
+      <c r="U62" s="91"/>
+      <c r="V62" s="91"/>
     </row>
     <row r="63" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="74"/>
@@ -5347,124 +5347,124 @@
       <c r="C64" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="D64" s="116"/>
-      <c r="E64" s="116"/>
-      <c r="F64" s="116"/>
-      <c r="G64" s="116"/>
-      <c r="H64" s="116"/>
-      <c r="I64" s="116"/>
-      <c r="J64" s="116"/>
-      <c r="K64" s="116"/>
-      <c r="L64" s="116"/>
-      <c r="M64" s="116"/>
-      <c r="N64" s="116"/>
-      <c r="O64" s="116"/>
-      <c r="P64" s="116"/>
-      <c r="Q64" s="116"/>
-      <c r="R64" s="116"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="89"/>
+      <c r="G64" s="89"/>
+      <c r="H64" s="89"/>
+      <c r="I64" s="89"/>
+      <c r="J64" s="89"/>
+      <c r="K64" s="89"/>
+      <c r="L64" s="89"/>
+      <c r="M64" s="89"/>
+      <c r="N64" s="89"/>
+      <c r="O64" s="89"/>
+      <c r="P64" s="89"/>
+      <c r="Q64" s="89"/>
+      <c r="R64" s="89"/>
       <c r="S64" s="64"/>
-      <c r="T64" s="108"/>
-      <c r="U64" s="109"/>
-      <c r="V64" s="110"/>
+      <c r="T64" s="85"/>
+      <c r="U64" s="86"/>
+      <c r="V64" s="87"/>
     </row>
     <row r="65" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
-      <c r="D65" s="116"/>
-      <c r="E65" s="116"/>
-      <c r="F65" s="116"/>
-      <c r="G65" s="116"/>
-      <c r="H65" s="116"/>
-      <c r="I65" s="116"/>
-      <c r="J65" s="116"/>
-      <c r="K65" s="116"/>
-      <c r="L65" s="116"/>
-      <c r="M65" s="116"/>
-      <c r="N65" s="116"/>
-      <c r="O65" s="116"/>
-      <c r="P65" s="116"/>
-      <c r="Q65" s="116"/>
-      <c r="R65" s="116"/>
+      <c r="D65" s="89"/>
+      <c r="E65" s="89"/>
+      <c r="F65" s="89"/>
+      <c r="G65" s="89"/>
+      <c r="H65" s="89"/>
+      <c r="I65" s="89"/>
+      <c r="J65" s="89"/>
+      <c r="K65" s="89"/>
+      <c r="L65" s="89"/>
+      <c r="M65" s="89"/>
+      <c r="N65" s="89"/>
+      <c r="O65" s="89"/>
+      <c r="P65" s="89"/>
+      <c r="Q65" s="89"/>
+      <c r="R65" s="89"/>
       <c r="S65" s="64"/>
-      <c r="T65" s="108"/>
-      <c r="U65" s="109"/>
-      <c r="V65" s="110"/>
+      <c r="T65" s="85"/>
+      <c r="U65" s="86"/>
+      <c r="V65" s="87"/>
     </row>
     <row r="66" spans="1:22" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
-      <c r="D66" s="116"/>
-      <c r="E66" s="116"/>
-      <c r="F66" s="116"/>
-      <c r="G66" s="116"/>
-      <c r="H66" s="116"/>
-      <c r="I66" s="116"/>
-      <c r="J66" s="116"/>
-      <c r="K66" s="116"/>
-      <c r="L66" s="116"/>
-      <c r="M66" s="116"/>
-      <c r="N66" s="116"/>
-      <c r="O66" s="116"/>
-      <c r="P66" s="116"/>
-      <c r="Q66" s="116"/>
-      <c r="R66" s="116"/>
+      <c r="D66" s="89"/>
+      <c r="E66" s="89"/>
+      <c r="F66" s="89"/>
+      <c r="G66" s="89"/>
+      <c r="H66" s="89"/>
+      <c r="I66" s="89"/>
+      <c r="J66" s="89"/>
+      <c r="K66" s="89"/>
+      <c r="L66" s="89"/>
+      <c r="M66" s="89"/>
+      <c r="N66" s="89"/>
+      <c r="O66" s="89"/>
+      <c r="P66" s="89"/>
+      <c r="Q66" s="89"/>
+      <c r="R66" s="89"/>
       <c r="S66" s="64"/>
-      <c r="T66" s="108"/>
-      <c r="U66" s="109"/>
-      <c r="V66" s="110"/>
+      <c r="T66" s="85"/>
+      <c r="U66" s="86"/>
+      <c r="V66" s="87"/>
     </row>
     <row r="67" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
-      <c r="D67" s="116"/>
-      <c r="E67" s="116"/>
-      <c r="F67" s="116"/>
-      <c r="G67" s="116"/>
-      <c r="H67" s="116"/>
-      <c r="I67" s="116"/>
-      <c r="J67" s="116"/>
-      <c r="K67" s="116"/>
-      <c r="L67" s="116"/>
-      <c r="M67" s="116"/>
-      <c r="N67" s="116"/>
-      <c r="O67" s="116"/>
-      <c r="P67" s="116"/>
-      <c r="Q67" s="116"/>
-      <c r="R67" s="116"/>
+      <c r="D67" s="89"/>
+      <c r="E67" s="89"/>
+      <c r="F67" s="89"/>
+      <c r="G67" s="89"/>
+      <c r="H67" s="89"/>
+      <c r="I67" s="89"/>
+      <c r="J67" s="89"/>
+      <c r="K67" s="89"/>
+      <c r="L67" s="89"/>
+      <c r="M67" s="89"/>
+      <c r="N67" s="89"/>
+      <c r="O67" s="89"/>
+      <c r="P67" s="89"/>
+      <c r="Q67" s="89"/>
+      <c r="R67" s="89"/>
       <c r="S67" s="64"/>
-      <c r="T67" s="108"/>
-      <c r="U67" s="109"/>
-      <c r="V67" s="110"/>
+      <c r="T67" s="85"/>
+      <c r="U67" s="86"/>
+      <c r="V67" s="87"/>
     </row>
     <row r="71" spans="1:22" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="92" t="s">
+      <c r="B71" s="117" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="93"/>
-      <c r="D71" s="91" t="s">
+      <c r="C71" s="118"/>
+      <c r="D71" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="E71" s="91"/>
-      <c r="F71" s="91"/>
-      <c r="G71" s="91"/>
-      <c r="H71" s="91"/>
-      <c r="I71" s="91"/>
-      <c r="J71" s="91"/>
-      <c r="K71" s="91"/>
-      <c r="L71" s="91"/>
-      <c r="M71" s="91"/>
-      <c r="N71" s="91"/>
-      <c r="O71" s="91"/>
-      <c r="P71" s="91"/>
-      <c r="Q71" s="91"/>
-      <c r="R71" s="91"/>
+      <c r="E71" s="116"/>
+      <c r="F71" s="116"/>
+      <c r="G71" s="116"/>
+      <c r="H71" s="116"/>
+      <c r="I71" s="116"/>
+      <c r="J71" s="116"/>
+      <c r="K71" s="116"/>
+      <c r="L71" s="116"/>
+      <c r="M71" s="116"/>
+      <c r="N71" s="116"/>
+      <c r="O71" s="116"/>
+      <c r="P71" s="116"/>
+      <c r="Q71" s="116"/>
+      <c r="R71" s="116"/>
     </row>
     <row r="72" spans="1:22" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="92"/>
-      <c r="C72" s="93"/>
+      <c r="B72" s="117"/>
+      <c r="C72" s="118"/>
       <c r="D72" s="78" t="s">
         <v>139</v>
       </c>
@@ -5502,8 +5502,8 @@
       <c r="R72" s="78"/>
     </row>
     <row r="73" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="92"/>
-      <c r="C73" s="93"/>
+      <c r="B73" s="117"/>
+      <c r="C73" s="118"/>
       <c r="D73" s="78" t="s">
         <v>149</v>
       </c>
@@ -5526,8 +5526,8 @@
       <c r="R73" s="78"/>
     </row>
     <row r="74" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="92"/>
-      <c r="C74" s="93"/>
+      <c r="B74" s="117"/>
+      <c r="C74" s="118"/>
       <c r="D74" s="78" t="s">
         <v>150</v>
       </c>
@@ -5550,8 +5550,8 @@
       <c r="R74" s="78"/>
     </row>
     <row r="75" spans="1:22" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="92"/>
-      <c r="C75" s="93"/>
+      <c r="B75" s="117"/>
+      <c r="C75" s="118"/>
       <c r="D75" s="78" t="s">
         <v>151</v>
       </c>
@@ -5608,21 +5608,21 @@
       <c r="B79" s="79"/>
       <c r="C79" s="79"/>
       <c r="D79" s="79"/>
-      <c r="E79" s="85" t="s">
+      <c r="E79" s="110" t="s">
         <v>152</v>
       </c>
-      <c r="F79" s="85"/>
-      <c r="G79" s="86"/>
-      <c r="H79" s="85" t="s">
+      <c r="F79" s="110"/>
+      <c r="G79" s="111"/>
+      <c r="H79" s="110" t="s">
         <v>172</v>
       </c>
-      <c r="I79" s="85"/>
-      <c r="J79" s="85"/>
-      <c r="K79" s="87" t="s">
+      <c r="I79" s="110"/>
+      <c r="J79" s="110"/>
+      <c r="K79" s="112" t="s">
         <v>173</v>
       </c>
-      <c r="L79" s="88"/>
-      <c r="M79" s="88"/>
+      <c r="L79" s="113"/>
+      <c r="M79" s="113"/>
       <c r="N79" s="80"/>
       <c r="O79" s="80"/>
       <c r="P79" s="80"/>
@@ -5631,15 +5631,15 @@
       <c r="B80" s="79"/>
       <c r="C80" s="79"/>
       <c r="D80" s="79"/>
-      <c r="E80" s="85"/>
-      <c r="F80" s="85"/>
-      <c r="G80" s="86"/>
-      <c r="H80" s="85"/>
-      <c r="I80" s="85"/>
-      <c r="J80" s="85"/>
-      <c r="K80" s="87"/>
-      <c r="L80" s="88"/>
-      <c r="M80" s="88"/>
+      <c r="E80" s="110"/>
+      <c r="F80" s="110"/>
+      <c r="G80" s="111"/>
+      <c r="H80" s="110"/>
+      <c r="I80" s="110"/>
+      <c r="J80" s="110"/>
+      <c r="K80" s="112"/>
+      <c r="L80" s="113"/>
+      <c r="M80" s="113"/>
       <c r="N80" s="80"/>
       <c r="O80" s="80"/>
       <c r="P80" s="80"/>
@@ -5648,15 +5648,15 @@
       <c r="B81" s="79"/>
       <c r="C81" s="79"/>
       <c r="D81" s="79"/>
-      <c r="E81" s="85"/>
-      <c r="F81" s="85"/>
-      <c r="G81" s="86"/>
-      <c r="H81" s="85"/>
-      <c r="I81" s="85"/>
-      <c r="J81" s="85"/>
-      <c r="K81" s="87"/>
-      <c r="L81" s="88"/>
-      <c r="M81" s="88"/>
+      <c r="E81" s="110"/>
+      <c r="F81" s="110"/>
+      <c r="G81" s="111"/>
+      <c r="H81" s="110"/>
+      <c r="I81" s="110"/>
+      <c r="J81" s="110"/>
+      <c r="K81" s="112"/>
+      <c r="L81" s="113"/>
+      <c r="M81" s="113"/>
       <c r="N81" s="80"/>
       <c r="O81" s="80"/>
       <c r="P81" s="80"/>
@@ -5665,15 +5665,15 @@
       <c r="B82" s="79"/>
       <c r="C82" s="79"/>
       <c r="D82" s="79"/>
-      <c r="E82" s="85"/>
-      <c r="F82" s="85"/>
-      <c r="G82" s="86"/>
-      <c r="H82" s="85"/>
-      <c r="I82" s="85"/>
-      <c r="J82" s="85"/>
-      <c r="K82" s="89"/>
-      <c r="L82" s="90"/>
-      <c r="M82" s="90"/>
+      <c r="E82" s="110"/>
+      <c r="F82" s="110"/>
+      <c r="G82" s="111"/>
+      <c r="H82" s="110"/>
+      <c r="I82" s="110"/>
+      <c r="J82" s="110"/>
+      <c r="K82" s="114"/>
+      <c r="L82" s="115"/>
+      <c r="M82" s="115"/>
       <c r="N82" s="80"/>
       <c r="O82" s="80"/>
       <c r="P82" s="80"/>
@@ -6495,7 +6495,9 @@
       <c r="D119" s="79"/>
       <c r="E119" s="82"/>
       <c r="F119" s="82"/>
-      <c r="G119" s="82"/>
+      <c r="G119" s="82">
+        <v>166.316</v>
+      </c>
       <c r="H119" s="82"/>
       <c r="I119" s="82"/>
       <c r="J119" s="82"/>
@@ -7086,6 +7088,67 @@
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="B71:C75"/>
+    <mergeCell ref="J57:O58"/>
+    <mergeCell ref="T55:V58"/>
+    <mergeCell ref="E79:G82"/>
+    <mergeCell ref="H79:J82"/>
+    <mergeCell ref="K79:M82"/>
+    <mergeCell ref="D71:R71"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="A16:V16"/>
+    <mergeCell ref="A37:R37"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="M38:Q38"/>
+    <mergeCell ref="H59:I59"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A57:C58"/>
+    <mergeCell ref="F57:G58"/>
+    <mergeCell ref="H57:I58"/>
+    <mergeCell ref="D57:E58"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="T64:V64"/>
+    <mergeCell ref="P62:S62"/>
+    <mergeCell ref="A55:S56"/>
+    <mergeCell ref="P57:S58"/>
+    <mergeCell ref="P59:S59"/>
+    <mergeCell ref="P60:S60"/>
+    <mergeCell ref="P61:S61"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="J60:O60"/>
+    <mergeCell ref="J61:O61"/>
+    <mergeCell ref="J62:O62"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H64:I64"/>
     <mergeCell ref="T65:V65"/>
     <mergeCell ref="T67:V67"/>
     <mergeCell ref="T66:V66"/>
@@ -7102,67 +7165,6 @@
     <mergeCell ref="T61:V61"/>
     <mergeCell ref="T62:V62"/>
     <mergeCell ref="J64:O64"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="T64:V64"/>
-    <mergeCell ref="P62:S62"/>
-    <mergeCell ref="A55:S56"/>
-    <mergeCell ref="P57:S58"/>
-    <mergeCell ref="P59:S59"/>
-    <mergeCell ref="P60:S60"/>
-    <mergeCell ref="P61:S61"/>
-    <mergeCell ref="J59:O59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="J60:O60"/>
-    <mergeCell ref="J61:O61"/>
-    <mergeCell ref="J62:O62"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A57:C58"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="A16:V16"/>
-    <mergeCell ref="A37:R37"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="M38:Q38"/>
-    <mergeCell ref="F57:G58"/>
-    <mergeCell ref="H57:I58"/>
-    <mergeCell ref="D57:E58"/>
-    <mergeCell ref="J57:O58"/>
-    <mergeCell ref="T55:V58"/>
-    <mergeCell ref="E79:G82"/>
-    <mergeCell ref="H79:J82"/>
-    <mergeCell ref="K79:M82"/>
-    <mergeCell ref="D71:R71"/>
-    <mergeCell ref="B71:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>